<commit_message>
Changed Dates on Datasheets
Changed from 28.10.2015 to 12.5.2015
</commit_message>
<xml_diff>
--- a/Specification/240-0201-EMEL-CL00-0001 CABLE SCHEDULE/P-240 CABLE SCHEDULE 11.11.15.xlsx
+++ b/Specification/240-0201-EMEL-CL00-0001 CABLE SCHEDULE/P-240 CABLE SCHEDULE 11.11.15.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Work\Project Documentation\P_240_Autocad_Docs\Specification\240-0201-EMEL-CL00-0001 CABLE SCHEDULE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
@@ -97,12 +102,12 @@
     <definedName name="Y">#REF!</definedName>
     <definedName name="zq_syst">'[3]CASE A1 CPP'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="298">
   <si>
     <t>:</t>
   </si>
@@ -990,9 +995,6 @@
   </si>
   <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>28/10/2015</t>
   </si>
   <si>
     <t>ISSUED FOR APPROVAL</t>
@@ -1009,7 +1011,7 @@
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="General_)"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="166" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="168" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -2468,11 +2470,77 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="43" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="46" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="44" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2516,83 +2584,52 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="43" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="46" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="44" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="2" borderId="43" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="2" borderId="44" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2603,14 +2640,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2621,66 +2658,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2705,15 +2704,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2723,6 +2713,15 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2732,74 +2731,77 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="15" fillId="2" borderId="43" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="15" fillId="2" borderId="44" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -3084,8 +3086,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7604752" y="102144"/>
-          <a:ext cx="977273" cy="726531"/>
+          <a:off x="7814302" y="102144"/>
+          <a:ext cx="1015373" cy="726531"/>
           <a:chOff x="7337307" y="99264"/>
           <a:chExt cx="684810" cy="511264"/>
         </a:xfrm>
@@ -4302,7 +4304,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4337,7 +4339,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4549,8 +4551,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S44" sqref="S44"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4589,94 +4591,94 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="224"/>
-      <c r="C2" s="225"/>
-      <c r="D2" s="225"/>
-      <c r="E2" s="225"/>
-      <c r="F2" s="225"/>
-      <c r="G2" s="226"/>
-      <c r="H2" s="230" t="s">
+      <c r="B2" s="213"/>
+      <c r="C2" s="214"/>
+      <c r="D2" s="214"/>
+      <c r="E2" s="214"/>
+      <c r="F2" s="214"/>
+      <c r="G2" s="215"/>
+      <c r="H2" s="219" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="231"/>
-      <c r="J2" s="231"/>
-      <c r="K2" s="231"/>
-      <c r="L2" s="231"/>
-      <c r="M2" s="231"/>
-      <c r="N2" s="231"/>
-      <c r="O2" s="232"/>
+      <c r="I2" s="220"/>
+      <c r="J2" s="220"/>
+      <c r="K2" s="220"/>
+      <c r="L2" s="220"/>
+      <c r="M2" s="220"/>
+      <c r="N2" s="220"/>
+      <c r="O2" s="221"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="227"/>
-      <c r="C3" s="228"/>
-      <c r="D3" s="228"/>
-      <c r="E3" s="228"/>
-      <c r="F3" s="228"/>
-      <c r="G3" s="229"/>
-      <c r="H3" s="233" t="s">
+      <c r="B3" s="216"/>
+      <c r="C3" s="217"/>
+      <c r="D3" s="217"/>
+      <c r="E3" s="217"/>
+      <c r="F3" s="217"/>
+      <c r="G3" s="218"/>
+      <c r="H3" s="222" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="234"/>
-      <c r="J3" s="234"/>
-      <c r="K3" s="234"/>
-      <c r="L3" s="234"/>
-      <c r="M3" s="234"/>
-      <c r="N3" s="234"/>
-      <c r="O3" s="235"/>
+      <c r="I3" s="223"/>
+      <c r="J3" s="223"/>
+      <c r="K3" s="223"/>
+      <c r="L3" s="223"/>
+      <c r="M3" s="223"/>
+      <c r="N3" s="223"/>
+      <c r="O3" s="224"/>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="227"/>
-      <c r="C4" s="228"/>
-      <c r="D4" s="228"/>
-      <c r="E4" s="228"/>
-      <c r="F4" s="228"/>
-      <c r="G4" s="229"/>
-      <c r="H4" s="233" t="s">
+      <c r="B4" s="216"/>
+      <c r="C4" s="217"/>
+      <c r="D4" s="217"/>
+      <c r="E4" s="217"/>
+      <c r="F4" s="217"/>
+      <c r="G4" s="218"/>
+      <c r="H4" s="222" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="234"/>
-      <c r="J4" s="234"/>
-      <c r="K4" s="234"/>
-      <c r="L4" s="234"/>
-      <c r="M4" s="234"/>
-      <c r="N4" s="234"/>
-      <c r="O4" s="235"/>
+      <c r="I4" s="223"/>
+      <c r="J4" s="223"/>
+      <c r="K4" s="223"/>
+      <c r="L4" s="223"/>
+      <c r="M4" s="223"/>
+      <c r="N4" s="223"/>
+      <c r="O4" s="224"/>
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="227"/>
-      <c r="C5" s="228"/>
-      <c r="D5" s="228"/>
-      <c r="E5" s="228"/>
-      <c r="F5" s="228"/>
-      <c r="G5" s="229"/>
-      <c r="H5" s="236" t="s">
+      <c r="B5" s="216"/>
+      <c r="C5" s="217"/>
+      <c r="D5" s="217"/>
+      <c r="E5" s="217"/>
+      <c r="F5" s="217"/>
+      <c r="G5" s="218"/>
+      <c r="H5" s="225" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="237"/>
-      <c r="J5" s="237"/>
-      <c r="K5" s="237"/>
-      <c r="L5" s="237"/>
-      <c r="M5" s="237"/>
-      <c r="N5" s="237"/>
-      <c r="O5" s="238"/>
+      <c r="I5" s="226"/>
+      <c r="J5" s="226"/>
+      <c r="K5" s="226"/>
+      <c r="L5" s="226"/>
+      <c r="M5" s="226"/>
+      <c r="N5" s="226"/>
+      <c r="O5" s="227"/>
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
-      <c r="B6" s="210" t="s">
+      <c r="B6" s="232" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="211"/>
-      <c r="D6" s="211"/>
-      <c r="E6" s="211"/>
-      <c r="F6" s="211"/>
-      <c r="G6" s="212"/>
+      <c r="C6" s="233"/>
+      <c r="D6" s="233"/>
+      <c r="E6" s="233"/>
+      <c r="F6" s="233"/>
+      <c r="G6" s="234"/>
       <c r="H6" s="6"/>
       <c r="I6" s="7"/>
       <c r="J6" s="8"/>
@@ -4689,12 +4691,12 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="213"/>
-      <c r="C7" s="211"/>
-      <c r="D7" s="211"/>
-      <c r="E7" s="211"/>
-      <c r="F7" s="211"/>
-      <c r="G7" s="212"/>
+      <c r="B7" s="235"/>
+      <c r="C7" s="233"/>
+      <c r="D7" s="233"/>
+      <c r="E7" s="233"/>
+      <c r="F7" s="233"/>
+      <c r="G7" s="234"/>
       <c r="H7" s="10" t="s">
         <v>5</v>
       </c>
@@ -4713,12 +4715,12 @@
     </row>
     <row r="8" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="214"/>
-      <c r="C8" s="215"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="216"/>
+      <c r="B8" s="236"/>
+      <c r="C8" s="237"/>
+      <c r="D8" s="237"/>
+      <c r="E8" s="237"/>
+      <c r="F8" s="237"/>
+      <c r="G8" s="238"/>
       <c r="H8" s="16" t="s">
         <v>8</v>
       </c>
@@ -4757,22 +4759,22 @@
     </row>
     <row r="10" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
-      <c r="B10" s="217" t="s">
+      <c r="B10" s="239" t="s">
         <v>267</v>
       </c>
-      <c r="C10" s="218"/>
-      <c r="D10" s="218"/>
-      <c r="E10" s="218"/>
-      <c r="F10" s="218"/>
-      <c r="G10" s="218"/>
-      <c r="H10" s="218"/>
-      <c r="I10" s="218"/>
-      <c r="J10" s="218"/>
-      <c r="K10" s="218"/>
-      <c r="L10" s="218"/>
-      <c r="M10" s="218"/>
-      <c r="N10" s="218"/>
-      <c r="O10" s="219"/>
+      <c r="C10" s="240"/>
+      <c r="D10" s="240"/>
+      <c r="E10" s="240"/>
+      <c r="F10" s="240"/>
+      <c r="G10" s="240"/>
+      <c r="H10" s="240"/>
+      <c r="I10" s="240"/>
+      <c r="J10" s="240"/>
+      <c r="K10" s="240"/>
+      <c r="L10" s="240"/>
+      <c r="M10" s="240"/>
+      <c r="N10" s="240"/>
+      <c r="O10" s="241"/>
       <c r="P10" s="21"/>
     </row>
     <row r="11" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4824,12 +4826,12 @@
       <c r="J13" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="220" t="s">
+      <c r="K13" s="242" t="s">
         <v>289</v>
       </c>
-      <c r="L13" s="220"/>
-      <c r="M13" s="220"/>
-      <c r="N13" s="221"/>
+      <c r="L13" s="242"/>
+      <c r="M13" s="242"/>
+      <c r="N13" s="243"/>
       <c r="O13" s="31"/>
       <c r="P13" s="21"/>
     </row>
@@ -5518,8 +5520,8 @@
       <c r="K49" s="55"/>
       <c r="L49" s="52"/>
       <c r="M49" s="52"/>
-      <c r="N49" s="222"/>
-      <c r="O49" s="223"/>
+      <c r="N49" s="244"/>
+      <c r="O49" s="245"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B50" s="56"/>
@@ -5534,8 +5536,8 @@
       <c r="K50" s="61"/>
       <c r="L50" s="59"/>
       <c r="M50" s="59"/>
-      <c r="N50" s="204"/>
-      <c r="O50" s="205"/>
+      <c r="N50" s="211"/>
+      <c r="O50" s="212"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B51" s="62"/>
@@ -5550,8 +5552,8 @@
       <c r="K51" s="61"/>
       <c r="L51" s="59"/>
       <c r="M51" s="59"/>
-      <c r="N51" s="204"/>
-      <c r="O51" s="205"/>
+      <c r="N51" s="211"/>
+      <c r="O51" s="212"/>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B52" s="62"/>
@@ -5566,8 +5568,8 @@
       <c r="K52" s="61"/>
       <c r="L52" s="59"/>
       <c r="M52" s="59"/>
-      <c r="N52" s="204"/>
-      <c r="O52" s="205"/>
+      <c r="N52" s="211"/>
+      <c r="O52" s="212"/>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B53" s="62"/>
@@ -5582,8 +5584,8 @@
       <c r="K53" s="61"/>
       <c r="L53" s="59"/>
       <c r="M53" s="59"/>
-      <c r="N53" s="204"/>
-      <c r="O53" s="205"/>
+      <c r="N53" s="211"/>
+      <c r="O53" s="212"/>
     </row>
     <row r="54" spans="2:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B54" s="66"/>
@@ -5598,38 +5600,38 @@
       <c r="K54" s="72"/>
       <c r="L54" s="69"/>
       <c r="M54" s="69"/>
-      <c r="N54" s="206"/>
-      <c r="O54" s="207"/>
+      <c r="N54" s="228"/>
+      <c r="O54" s="229"/>
     </row>
     <row r="55" spans="2:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B55" s="66" t="s">
         <v>295</v>
       </c>
-      <c r="C55" s="246" t="s">
-        <v>296</v>
-      </c>
-      <c r="D55" s="247"/>
+      <c r="C55" s="325">
+        <v>42136</v>
+      </c>
+      <c r="D55" s="326"/>
       <c r="E55" s="69">
         <v>4</v>
       </c>
-      <c r="F55" s="243" t="s">
-        <v>297</v>
-      </c>
-      <c r="G55" s="244"/>
-      <c r="H55" s="244"/>
-      <c r="I55" s="244"/>
-      <c r="J55" s="244"/>
-      <c r="K55" s="245"/>
+      <c r="F55" s="208" t="s">
+        <v>296</v>
+      </c>
+      <c r="G55" s="209"/>
+      <c r="H55" s="209"/>
+      <c r="I55" s="209"/>
+      <c r="J55" s="209"/>
+      <c r="K55" s="210"/>
       <c r="L55" s="73" t="s">
         <v>292</v>
       </c>
       <c r="M55" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="N55" s="208" t="s">
+      <c r="N55" s="230" t="s">
         <v>293</v>
       </c>
-      <c r="O55" s="209"/>
+      <c r="O55" s="231"/>
     </row>
     <row r="56" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B56" s="74" t="s">
@@ -5642,37 +5644,27 @@
       <c r="E56" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="F56" s="239" t="s">
+      <c r="F56" s="204" t="s">
         <v>22</v>
       </c>
-      <c r="G56" s="240"/>
-      <c r="H56" s="240"/>
-      <c r="I56" s="240"/>
-      <c r="J56" s="240"/>
-      <c r="K56" s="241"/>
+      <c r="G56" s="205"/>
+      <c r="H56" s="205"/>
+      <c r="I56" s="205"/>
+      <c r="J56" s="205"/>
+      <c r="K56" s="206"/>
       <c r="L56" s="77" t="s">
         <v>23</v>
       </c>
       <c r="M56" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="N56" s="239" t="s">
+      <c r="N56" s="204" t="s">
         <v>25</v>
       </c>
-      <c r="O56" s="242"/>
+      <c r="O56" s="207"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="F56:K56"/>
-    <mergeCell ref="N56:O56"/>
-    <mergeCell ref="F55:K55"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="N52:O52"/>
-    <mergeCell ref="B2:G5"/>
-    <mergeCell ref="H2:O2"/>
-    <mergeCell ref="H3:O3"/>
-    <mergeCell ref="H4:O4"/>
-    <mergeCell ref="H5:O5"/>
     <mergeCell ref="N51:O51"/>
     <mergeCell ref="N53:O53"/>
     <mergeCell ref="N54:O54"/>
@@ -5682,6 +5674,16 @@
     <mergeCell ref="K13:N13"/>
     <mergeCell ref="N49:O49"/>
     <mergeCell ref="N50:O50"/>
+    <mergeCell ref="B2:G5"/>
+    <mergeCell ref="H2:O2"/>
+    <mergeCell ref="H3:O3"/>
+    <mergeCell ref="H4:O4"/>
+    <mergeCell ref="H5:O5"/>
+    <mergeCell ref="F56:K56"/>
+    <mergeCell ref="N56:O56"/>
+    <mergeCell ref="F55:K55"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="N52:O52"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.25" top="0.5" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -5693,8 +5695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R568"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A67" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70:I70"/>
+    <sheetView view="pageLayout" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B138" sqref="B138:D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5725,10 +5727,10 @@
       <c r="C1" s="86"/>
       <c r="D1" s="86"/>
       <c r="E1" s="86"/>
-      <c r="F1" s="312" t="s">
+      <c r="F1" s="248" t="s">
         <v>252</v>
       </c>
-      <c r="G1" s="313"/>
+      <c r="G1" s="249"/>
       <c r="H1" s="86"/>
       <c r="I1" s="86"/>
       <c r="J1" s="86"/>
@@ -5743,8 +5745,8 @@
       <c r="C2" s="92"/>
       <c r="D2" s="92"/>
       <c r="E2" s="92"/>
-      <c r="F2" s="314"/>
-      <c r="G2" s="315"/>
+      <c r="F2" s="250"/>
+      <c r="G2" s="251"/>
       <c r="H2" s="123"/>
       <c r="I2" s="123"/>
       <c r="J2" s="123"/>
@@ -5761,8 +5763,8 @@
       <c r="C3" s="201"/>
       <c r="D3" s="201"/>
       <c r="E3" s="201"/>
-      <c r="F3" s="314"/>
-      <c r="G3" s="315"/>
+      <c r="F3" s="250"/>
+      <c r="G3" s="251"/>
       <c r="H3" s="124"/>
       <c r="I3" s="124"/>
       <c r="J3" s="124"/>
@@ -5778,8 +5780,8 @@
       <c r="C4" s="201"/>
       <c r="D4" s="201"/>
       <c r="E4" s="201"/>
-      <c r="F4" s="314"/>
-      <c r="G4" s="315"/>
+      <c r="F4" s="250"/>
+      <c r="G4" s="251"/>
       <c r="H4" s="125"/>
       <c r="I4" s="125"/>
       <c r="J4" s="125"/>
@@ -5795,8 +5797,8 @@
       <c r="C5" s="84"/>
       <c r="D5" s="84"/>
       <c r="E5" s="84"/>
-      <c r="F5" s="316"/>
-      <c r="G5" s="317"/>
+      <c r="F5" s="252"/>
+      <c r="G5" s="253"/>
       <c r="H5" s="126"/>
       <c r="I5" s="126"/>
       <c r="J5" s="126"/>
@@ -5809,105 +5811,105 @@
       <c r="R5" s="89"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="310" t="s">
+      <c r="A6" s="246" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="311"/>
+      <c r="B6" s="247"/>
       <c r="C6" s="99"/>
-      <c r="D6" s="324" t="s">
+      <c r="D6" s="260" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="325"/>
-      <c r="F6" s="325"/>
-      <c r="G6" s="326"/>
+      <c r="E6" s="261"/>
+      <c r="F6" s="261"/>
+      <c r="G6" s="262"/>
       <c r="H6" s="174" t="s">
         <v>258</v>
       </c>
-      <c r="I6" s="265" t="s">
+      <c r="I6" s="310" t="s">
         <v>289</v>
       </c>
-      <c r="J6" s="266"/>
-      <c r="K6" s="266"/>
-      <c r="L6" s="267"/>
-      <c r="M6" s="268" t="s">
+      <c r="J6" s="311"/>
+      <c r="K6" s="311"/>
+      <c r="L6" s="312"/>
+      <c r="M6" s="313" t="s">
         <v>294</v>
       </c>
-      <c r="N6" s="269"/>
+      <c r="N6" s="314"/>
       <c r="O6" s="116"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="308" t="s">
+      <c r="A7" s="280" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="309"/>
+      <c r="B7" s="281"/>
       <c r="C7" s="99"/>
-      <c r="D7" s="321" t="s">
+      <c r="D7" s="257" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="322"/>
-      <c r="F7" s="322"/>
-      <c r="G7" s="323"/>
+      <c r="E7" s="258"/>
+      <c r="F7" s="258"/>
+      <c r="G7" s="259"/>
       <c r="H7" s="142" t="s">
         <v>259</v>
       </c>
-      <c r="I7" s="270"/>
-      <c r="J7" s="270"/>
-      <c r="K7" s="270"/>
-      <c r="L7" s="270"/>
-      <c r="M7" s="268"/>
-      <c r="N7" s="269"/>
+      <c r="I7" s="315"/>
+      <c r="J7" s="315"/>
+      <c r="K7" s="315"/>
+      <c r="L7" s="315"/>
+      <c r="M7" s="313"/>
+      <c r="N7" s="314"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="308" t="s">
+      <c r="A8" s="280" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="309"/>
+      <c r="B8" s="281"/>
       <c r="C8" s="99"/>
-      <c r="D8" s="321" t="s">
+      <c r="D8" s="257" t="s">
         <v>269</v>
       </c>
-      <c r="E8" s="322"/>
-      <c r="F8" s="322"/>
-      <c r="G8" s="323"/>
+      <c r="E8" s="258"/>
+      <c r="F8" s="258"/>
+      <c r="G8" s="259"/>
       <c r="H8" s="143" t="s">
         <v>255</v>
       </c>
-      <c r="I8" s="271" t="s">
+      <c r="I8" s="316" t="s">
         <v>256</v>
       </c>
-      <c r="J8" s="271"/>
-      <c r="K8" s="271"/>
-      <c r="L8" s="271"/>
-      <c r="M8" s="268"/>
-      <c r="N8" s="269"/>
+      <c r="J8" s="316"/>
+      <c r="K8" s="316"/>
+      <c r="L8" s="316"/>
+      <c r="M8" s="313"/>
+      <c r="N8" s="314"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="308" t="s">
+      <c r="A9" s="280" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="309"/>
+      <c r="B9" s="281"/>
       <c r="C9" s="99"/>
-      <c r="D9" s="318">
-        <v>240</v>
-      </c>
-      <c r="E9" s="319"/>
-      <c r="F9" s="319"/>
-      <c r="G9" s="320"/>
+      <c r="D9" s="254">
+        <v>240</v>
+      </c>
+      <c r="E9" s="255"/>
+      <c r="F9" s="255"/>
+      <c r="G9" s="256"/>
       <c r="H9" s="143" t="s">
         <v>257</v>
       </c>
-      <c r="I9" s="271" t="s">
+      <c r="I9" s="316" t="s">
         <v>256</v>
       </c>
-      <c r="J9" s="271"/>
-      <c r="K9" s="271"/>
-      <c r="L9" s="271"/>
+      <c r="J9" s="316"/>
+      <c r="K9" s="316"/>
+      <c r="L9" s="316"/>
       <c r="M9" s="98"/>
       <c r="N9" s="132"/>
     </row>
     <row r="10" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="300"/>
-      <c r="B10" s="301"/>
+      <c r="A10" s="272"/>
+      <c r="B10" s="273"/>
       <c r="C10" s="100"/>
       <c r="D10" s="201"/>
       <c r="E10" s="201"/>
@@ -5928,11 +5930,11 @@
       <c r="B11" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="302" t="s">
+      <c r="C11" s="274" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="303"/>
-      <c r="E11" s="304"/>
+      <c r="D11" s="275"/>
+      <c r="E11" s="276"/>
       <c r="F11" s="107" t="s">
         <v>234</v>
       </c>
@@ -5965,9 +5967,9 @@
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="134"/>
       <c r="B12" s="104"/>
-      <c r="C12" s="305"/>
-      <c r="D12" s="306"/>
-      <c r="E12" s="307"/>
+      <c r="C12" s="277"/>
+      <c r="D12" s="278"/>
+      <c r="E12" s="279"/>
       <c r="F12" s="201"/>
       <c r="G12" s="201"/>
       <c r="H12" s="103"/>
@@ -5986,11 +5988,11 @@
       <c r="B13" s="167" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="259" t="s">
+      <c r="C13" s="266" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="260"/>
-      <c r="E13" s="261"/>
+      <c r="D13" s="267"/>
+      <c r="E13" s="268"/>
       <c r="F13" s="167" t="s">
         <v>70</v>
       </c>
@@ -6027,11 +6029,11 @@
       <c r="B14" s="167" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="259" t="s">
+      <c r="C14" s="266" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="260"/>
-      <c r="E14" s="261"/>
+      <c r="D14" s="267"/>
+      <c r="E14" s="268"/>
       <c r="F14" s="167" t="s">
         <v>72</v>
       </c>
@@ -6068,11 +6070,11 @@
       <c r="B15" s="152" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="259" t="s">
+      <c r="C15" s="266" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="260"/>
-      <c r="E15" s="261"/>
+      <c r="D15" s="267"/>
+      <c r="E15" s="268"/>
       <c r="F15" s="167" t="s">
         <v>96</v>
       </c>
@@ -6109,11 +6111,11 @@
       <c r="B16" s="152" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="259" t="s">
+      <c r="C16" s="266" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="260"/>
-      <c r="E16" s="261"/>
+      <c r="D16" s="267"/>
+      <c r="E16" s="268"/>
       <c r="F16" s="167" t="s">
         <v>89</v>
       </c>
@@ -6121,7 +6123,7 @@
         <v>71</v>
       </c>
       <c r="H16" s="163" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I16" s="192"/>
       <c r="J16" s="188" t="s">
@@ -6144,11 +6146,11 @@
         <v>5</v>
       </c>
       <c r="B17" s="153"/>
-      <c r="C17" s="259" t="s">
+      <c r="C17" s="266" t="s">
         <v>98</v>
       </c>
-      <c r="D17" s="260"/>
-      <c r="E17" s="261"/>
+      <c r="D17" s="267"/>
+      <c r="E17" s="268"/>
       <c r="F17" s="154"/>
       <c r="G17" s="153"/>
       <c r="H17" s="163" t="s">
@@ -6179,11 +6181,11 @@
         <v>6</v>
       </c>
       <c r="B18" s="153"/>
-      <c r="C18" s="259" t="s">
+      <c r="C18" s="266" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="260"/>
-      <c r="E18" s="261"/>
+      <c r="D18" s="267"/>
+      <c r="E18" s="268"/>
       <c r="F18" s="154"/>
       <c r="G18" s="153"/>
       <c r="H18" s="163" t="s">
@@ -6214,11 +6216,11 @@
         <v>7</v>
       </c>
       <c r="B19" s="153"/>
-      <c r="C19" s="259" t="s">
+      <c r="C19" s="266" t="s">
         <v>104</v>
       </c>
-      <c r="D19" s="260"/>
-      <c r="E19" s="261"/>
+      <c r="D19" s="267"/>
+      <c r="E19" s="268"/>
       <c r="F19" s="154"/>
       <c r="G19" s="153"/>
       <c r="H19" s="163" t="s">
@@ -6249,11 +6251,11 @@
         <v>8</v>
       </c>
       <c r="B20" s="153"/>
-      <c r="C20" s="259" t="s">
+      <c r="C20" s="266" t="s">
         <v>105</v>
       </c>
-      <c r="D20" s="260"/>
-      <c r="E20" s="261"/>
+      <c r="D20" s="267"/>
+      <c r="E20" s="268"/>
       <c r="F20" s="154"/>
       <c r="G20" s="153"/>
       <c r="H20" s="163" t="s">
@@ -6284,11 +6286,11 @@
         <v>9</v>
       </c>
       <c r="B21" s="153"/>
-      <c r="C21" s="259" t="s">
+      <c r="C21" s="266" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="260"/>
-      <c r="E21" s="261"/>
+      <c r="D21" s="267"/>
+      <c r="E21" s="268"/>
       <c r="F21" s="154"/>
       <c r="G21" s="153"/>
       <c r="H21" s="163" t="s">
@@ -6321,11 +6323,11 @@
       <c r="B22" s="193" t="s">
         <v>107</v>
       </c>
-      <c r="C22" s="259" t="s">
+      <c r="C22" s="266" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="260"/>
-      <c r="E22" s="261"/>
+      <c r="D22" s="267"/>
+      <c r="E22" s="268"/>
       <c r="F22" s="163" t="s">
         <v>71</v>
       </c>
@@ -6362,11 +6364,11 @@
       <c r="B23" s="193" t="s">
         <v>109</v>
       </c>
-      <c r="C23" s="259" t="s">
+      <c r="C23" s="266" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="260"/>
-      <c r="E23" s="261"/>
+      <c r="D23" s="267"/>
+      <c r="E23" s="268"/>
       <c r="F23" s="163" t="s">
         <v>71</v>
       </c>
@@ -6403,11 +6405,11 @@
       <c r="B24" s="193" t="s">
         <v>110</v>
       </c>
-      <c r="C24" s="259" t="s">
+      <c r="C24" s="266" t="s">
         <v>108</v>
       </c>
-      <c r="D24" s="260"/>
-      <c r="E24" s="261"/>
+      <c r="D24" s="267"/>
+      <c r="E24" s="268"/>
       <c r="F24" s="163" t="s">
         <v>71</v>
       </c>
@@ -6442,11 +6444,11 @@
         <v>13</v>
       </c>
       <c r="B25" s="152"/>
-      <c r="C25" s="259" t="s">
+      <c r="C25" s="266" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="260"/>
-      <c r="E25" s="261"/>
+      <c r="D25" s="267"/>
+      <c r="E25" s="268"/>
       <c r="F25" s="163" t="s">
         <v>71</v>
       </c>
@@ -6481,11 +6483,11 @@
         <v>14</v>
       </c>
       <c r="B26" s="153"/>
-      <c r="C26" s="259" t="s">
+      <c r="C26" s="266" t="s">
         <v>114</v>
       </c>
-      <c r="D26" s="260"/>
-      <c r="E26" s="261"/>
+      <c r="D26" s="267"/>
+      <c r="E26" s="268"/>
       <c r="F26" s="163" t="s">
         <v>71</v>
       </c>
@@ -6516,17 +6518,17 @@
       <c r="O26" s="78"/>
     </row>
     <row r="27" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="250">
+      <c r="A27" s="263">
         <v>15</v>
       </c>
       <c r="B27" s="155" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="256" t="s">
+      <c r="C27" s="269" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="257"/>
-      <c r="E27" s="258"/>
+      <c r="D27" s="270"/>
+      <c r="E27" s="271"/>
       <c r="F27" s="167" t="s">
         <v>71</v>
       </c>
@@ -6557,15 +6559,15 @@
       <c r="O27" s="78"/>
     </row>
     <row r="28" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="252"/>
+      <c r="A28" s="265"/>
       <c r="B28" s="156" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="256" t="s">
+      <c r="C28" s="269" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="257"/>
-      <c r="E28" s="258"/>
+      <c r="D28" s="270"/>
+      <c r="E28" s="271"/>
       <c r="F28" s="167" t="s">
         <v>71</v>
       </c>
@@ -6596,17 +6598,17 @@
       <c r="O28" s="78"/>
     </row>
     <row r="29" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="250">
+      <c r="A29" s="263">
         <v>16</v>
       </c>
       <c r="B29" s="152" t="s">
         <v>118</v>
       </c>
-      <c r="C29" s="256" t="s">
+      <c r="C29" s="269" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="257"/>
-      <c r="E29" s="258"/>
+      <c r="D29" s="270"/>
+      <c r="E29" s="271"/>
       <c r="F29" s="167" t="s">
         <v>71</v>
       </c>
@@ -6635,15 +6637,15 @@
       <c r="O29" s="78"/>
     </row>
     <row r="30" spans="1:17" s="194" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="252"/>
+      <c r="A30" s="265"/>
       <c r="B30" s="198" t="s">
         <v>120</v>
       </c>
-      <c r="C30" s="256" t="s">
+      <c r="C30" s="269" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="257"/>
-      <c r="E30" s="258"/>
+      <c r="D30" s="270"/>
+      <c r="E30" s="271"/>
       <c r="F30" s="167" t="s">
         <v>71</v>
       </c>
@@ -6674,17 +6676,17 @@
       <c r="Q30" s="117"/>
     </row>
     <row r="31" spans="1:17" s="79" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="250">
+      <c r="A31" s="263">
         <v>17</v>
       </c>
       <c r="B31" s="156" t="s">
         <v>121</v>
       </c>
-      <c r="C31" s="256" t="s">
+      <c r="C31" s="269" t="s">
         <v>122</v>
       </c>
-      <c r="D31" s="257"/>
-      <c r="E31" s="258"/>
+      <c r="D31" s="270"/>
+      <c r="E31" s="271"/>
       <c r="F31" s="167" t="s">
         <v>71</v>
       </c>
@@ -6717,15 +6719,15 @@
       <c r="Q31" s="117"/>
     </row>
     <row r="32" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="252"/>
+      <c r="A32" s="265"/>
       <c r="B32" s="156" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="256" t="s">
+      <c r="C32" s="269" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="257"/>
-      <c r="E32" s="258"/>
+      <c r="D32" s="270"/>
+      <c r="E32" s="271"/>
       <c r="F32" s="167" t="s">
         <v>71</v>
       </c>
@@ -6756,17 +6758,17 @@
       <c r="O32" s="78"/>
     </row>
     <row r="33" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="250">
+      <c r="A33" s="263">
         <v>18</v>
       </c>
       <c r="B33" s="198" t="s">
         <v>206</v>
       </c>
-      <c r="C33" s="256" t="s">
+      <c r="C33" s="269" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="257"/>
-      <c r="E33" s="258"/>
+      <c r="D33" s="270"/>
+      <c r="E33" s="271"/>
       <c r="F33" s="167" t="s">
         <v>71</v>
       </c>
@@ -6795,15 +6797,15 @@
       <c r="O33" s="78"/>
     </row>
     <row r="34" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="252"/>
+      <c r="A34" s="265"/>
       <c r="B34" s="198" t="s">
         <v>207</v>
       </c>
-      <c r="C34" s="256" t="s">
+      <c r="C34" s="269" t="s">
         <v>124</v>
       </c>
-      <c r="D34" s="257"/>
-      <c r="E34" s="258"/>
+      <c r="D34" s="270"/>
+      <c r="E34" s="271"/>
       <c r="F34" s="167" t="s">
         <v>71</v>
       </c>
@@ -6832,17 +6834,17 @@
       <c r="O34" s="78"/>
     </row>
     <row r="35" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="250">
+      <c r="A35" s="263">
         <v>19</v>
       </c>
       <c r="B35" s="156" t="s">
         <v>125</v>
       </c>
-      <c r="C35" s="256" t="s">
+      <c r="C35" s="269" t="s">
         <v>126</v>
       </c>
-      <c r="D35" s="257"/>
-      <c r="E35" s="258"/>
+      <c r="D35" s="270"/>
+      <c r="E35" s="271"/>
       <c r="F35" s="167" t="s">
         <v>71</v>
       </c>
@@ -6873,15 +6875,15 @@
       <c r="O35" s="78"/>
     </row>
     <row r="36" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="252"/>
+      <c r="A36" s="265"/>
       <c r="B36" s="198" t="s">
         <v>128</v>
       </c>
-      <c r="C36" s="256" t="s">
+      <c r="C36" s="269" t="s">
         <v>129</v>
       </c>
-      <c r="D36" s="257"/>
-      <c r="E36" s="258"/>
+      <c r="D36" s="270"/>
+      <c r="E36" s="271"/>
       <c r="F36" s="167" t="s">
         <v>71</v>
       </c>
@@ -6910,17 +6912,17 @@
       <c r="O36" s="78"/>
     </row>
     <row r="37" spans="1:15" s="117" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="277">
+      <c r="A37" s="303">
         <v>20</v>
       </c>
       <c r="B37" s="156" t="s">
         <v>130</v>
       </c>
-      <c r="C37" s="256" t="s">
+      <c r="C37" s="269" t="s">
         <v>126</v>
       </c>
-      <c r="D37" s="257"/>
-      <c r="E37" s="258"/>
+      <c r="D37" s="270"/>
+      <c r="E37" s="271"/>
       <c r="F37" s="167" t="s">
         <v>71</v>
       </c>
@@ -6950,15 +6952,15 @@
       </c>
     </row>
     <row r="38" spans="1:15" s="117" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="278"/>
+      <c r="A38" s="304"/>
       <c r="B38" s="198" t="s">
         <v>131</v>
       </c>
-      <c r="C38" s="256" t="s">
+      <c r="C38" s="269" t="s">
         <v>129</v>
       </c>
-      <c r="D38" s="257"/>
-      <c r="E38" s="258"/>
+      <c r="D38" s="270"/>
+      <c r="E38" s="271"/>
       <c r="F38" s="167" t="s">
         <v>71</v>
       </c>
@@ -6986,17 +6988,17 @@
       <c r="N38" s="136"/>
     </row>
     <row r="39" spans="1:15" s="117" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="277">
+      <c r="A39" s="303">
         <v>21</v>
       </c>
       <c r="B39" s="156" t="s">
         <v>132</v>
       </c>
-      <c r="C39" s="256" t="s">
+      <c r="C39" s="269" t="s">
         <v>126</v>
       </c>
-      <c r="D39" s="257"/>
-      <c r="E39" s="258"/>
+      <c r="D39" s="270"/>
+      <c r="E39" s="271"/>
       <c r="F39" s="167" t="s">
         <v>71</v>
       </c>
@@ -7026,15 +7028,15 @@
       </c>
     </row>
     <row r="40" spans="1:15" s="117" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="278"/>
+      <c r="A40" s="304"/>
       <c r="B40" s="198" t="s">
         <v>133</v>
       </c>
-      <c r="C40" s="256" t="s">
+      <c r="C40" s="269" t="s">
         <v>129</v>
       </c>
-      <c r="D40" s="257"/>
-      <c r="E40" s="258"/>
+      <c r="D40" s="270"/>
+      <c r="E40" s="271"/>
       <c r="F40" s="167" t="s">
         <v>71</v>
       </c>
@@ -7062,17 +7064,17 @@
       <c r="N40" s="136"/>
     </row>
     <row r="41" spans="1:15" s="117" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="250">
+      <c r="A41" s="263">
         <v>22</v>
       </c>
       <c r="B41" s="156" t="s">
         <v>134</v>
       </c>
-      <c r="C41" s="256" t="s">
+      <c r="C41" s="269" t="s">
         <v>126</v>
       </c>
-      <c r="D41" s="257"/>
-      <c r="E41" s="258"/>
+      <c r="D41" s="270"/>
+      <c r="E41" s="271"/>
       <c r="F41" s="167" t="s">
         <v>71</v>
       </c>
@@ -7102,15 +7104,15 @@
       </c>
     </row>
     <row r="42" spans="1:15" s="79" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="252"/>
+      <c r="A42" s="265"/>
       <c r="B42" s="198" t="s">
         <v>135</v>
       </c>
-      <c r="C42" s="256" t="s">
+      <c r="C42" s="269" t="s">
         <v>129</v>
       </c>
-      <c r="D42" s="257"/>
-      <c r="E42" s="258"/>
+      <c r="D42" s="270"/>
+      <c r="E42" s="271"/>
       <c r="F42" s="167" t="s">
         <v>71</v>
       </c>
@@ -7138,17 +7140,17 @@
       <c r="N42" s="136"/>
     </row>
     <row r="43" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="250">
+      <c r="A43" s="263">
         <v>23</v>
       </c>
       <c r="B43" s="198" t="s">
         <v>136</v>
       </c>
-      <c r="C43" s="256" t="s">
+      <c r="C43" s="269" t="s">
         <v>137</v>
       </c>
-      <c r="D43" s="257"/>
-      <c r="E43" s="258"/>
+      <c r="D43" s="270"/>
+      <c r="E43" s="271"/>
       <c r="F43" s="167" t="s">
         <v>71</v>
       </c>
@@ -7179,15 +7181,15 @@
       <c r="O43" s="78"/>
     </row>
     <row r="44" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="252"/>
+      <c r="A44" s="265"/>
       <c r="B44" s="198" t="s">
         <v>138</v>
       </c>
-      <c r="C44" s="256" t="s">
+      <c r="C44" s="269" t="s">
         <v>139</v>
       </c>
-      <c r="D44" s="257"/>
-      <c r="E44" s="258"/>
+      <c r="D44" s="270"/>
+      <c r="E44" s="271"/>
       <c r="F44" s="167" t="s">
         <v>71</v>
       </c>
@@ -7216,17 +7218,17 @@
       <c r="O44" s="78"/>
     </row>
     <row r="45" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="250">
+      <c r="A45" s="263">
         <v>24</v>
       </c>
       <c r="B45" s="198" t="s">
         <v>140</v>
       </c>
-      <c r="C45" s="256" t="s">
+      <c r="C45" s="269" t="s">
         <v>137</v>
       </c>
-      <c r="D45" s="257"/>
-      <c r="E45" s="258"/>
+      <c r="D45" s="270"/>
+      <c r="E45" s="271"/>
       <c r="F45" s="167" t="s">
         <v>71</v>
       </c>
@@ -7257,15 +7259,15 @@
       <c r="O45" s="78"/>
     </row>
     <row r="46" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="252"/>
+      <c r="A46" s="265"/>
       <c r="B46" s="198" t="s">
         <v>141</v>
       </c>
-      <c r="C46" s="256" t="s">
+      <c r="C46" s="269" t="s">
         <v>139</v>
       </c>
-      <c r="D46" s="257"/>
-      <c r="E46" s="258"/>
+      <c r="D46" s="270"/>
+      <c r="E46" s="271"/>
       <c r="F46" s="167" t="s">
         <v>71</v>
       </c>
@@ -7294,17 +7296,17 @@
       <c r="O46" s="78"/>
     </row>
     <row r="47" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="250">
+      <c r="A47" s="263">
         <v>25</v>
       </c>
       <c r="B47" s="198" t="s">
         <v>142</v>
       </c>
-      <c r="C47" s="256" t="s">
+      <c r="C47" s="269" t="s">
         <v>137</v>
       </c>
-      <c r="D47" s="257"/>
-      <c r="E47" s="258"/>
+      <c r="D47" s="270"/>
+      <c r="E47" s="271"/>
       <c r="F47" s="167" t="s">
         <v>71</v>
       </c>
@@ -7335,15 +7337,15 @@
       <c r="O47" s="78"/>
     </row>
     <row r="48" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="252"/>
+      <c r="A48" s="265"/>
       <c r="B48" s="198" t="s">
         <v>143</v>
       </c>
-      <c r="C48" s="256" t="s">
+      <c r="C48" s="269" t="s">
         <v>139</v>
       </c>
-      <c r="D48" s="257"/>
-      <c r="E48" s="258"/>
+      <c r="D48" s="270"/>
+      <c r="E48" s="271"/>
       <c r="F48" s="167" t="s">
         <v>71</v>
       </c>
@@ -7372,17 +7374,17 @@
       <c r="O48" s="78"/>
     </row>
     <row r="49" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="250">
+      <c r="A49" s="263">
         <v>26</v>
       </c>
       <c r="B49" s="198" t="s">
         <v>144</v>
       </c>
-      <c r="C49" s="256" t="s">
+      <c r="C49" s="269" t="s">
         <v>137</v>
       </c>
-      <c r="D49" s="257"/>
-      <c r="E49" s="258"/>
+      <c r="D49" s="270"/>
+      <c r="E49" s="271"/>
       <c r="F49" s="167" t="s">
         <v>71</v>
       </c>
@@ -7413,15 +7415,15 @@
       <c r="O49" s="78"/>
     </row>
     <row r="50" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="252"/>
+      <c r="A50" s="265"/>
       <c r="B50" s="198" t="s">
         <v>145</v>
       </c>
-      <c r="C50" s="256" t="s">
+      <c r="C50" s="269" t="s">
         <v>139</v>
       </c>
-      <c r="D50" s="257"/>
-      <c r="E50" s="258"/>
+      <c r="D50" s="270"/>
+      <c r="E50" s="271"/>
       <c r="F50" s="167" t="s">
         <v>71</v>
       </c>
@@ -7450,17 +7452,17 @@
       <c r="O50" s="78"/>
     </row>
     <row r="51" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="250">
+      <c r="A51" s="263">
         <v>27</v>
       </c>
       <c r="B51" s="198" t="s">
         <v>146</v>
       </c>
-      <c r="C51" s="256" t="s">
+      <c r="C51" s="269" t="s">
         <v>147</v>
       </c>
-      <c r="D51" s="257"/>
-      <c r="E51" s="258"/>
+      <c r="D51" s="270"/>
+      <c r="E51" s="271"/>
       <c r="F51" s="167" t="s">
         <v>71</v>
       </c>
@@ -7491,15 +7493,15 @@
       <c r="O51" s="78"/>
     </row>
     <row r="52" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="252"/>
+      <c r="A52" s="265"/>
       <c r="B52" s="198" t="s">
         <v>148</v>
       </c>
-      <c r="C52" s="256" t="s">
+      <c r="C52" s="269" t="s">
         <v>149</v>
       </c>
-      <c r="D52" s="257"/>
-      <c r="E52" s="258"/>
+      <c r="D52" s="270"/>
+      <c r="E52" s="271"/>
       <c r="F52" s="167" t="s">
         <v>71</v>
       </c>
@@ -7528,17 +7530,17 @@
       <c r="O52" s="78"/>
     </row>
     <row r="53" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="275">
+      <c r="A53" s="305">
         <v>28</v>
       </c>
       <c r="B53" s="198" t="s">
         <v>150</v>
       </c>
-      <c r="C53" s="256" t="s">
+      <c r="C53" s="269" t="s">
         <v>147</v>
       </c>
-      <c r="D53" s="257"/>
-      <c r="E53" s="258"/>
+      <c r="D53" s="270"/>
+      <c r="E53" s="271"/>
       <c r="F53" s="167" t="s">
         <v>71</v>
       </c>
@@ -7569,15 +7571,15 @@
       <c r="O53" s="78"/>
     </row>
     <row r="54" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="276"/>
+      <c r="A54" s="306"/>
       <c r="B54" s="198" t="s">
         <v>151</v>
       </c>
-      <c r="C54" s="256" t="s">
+      <c r="C54" s="269" t="s">
         <v>149</v>
       </c>
-      <c r="D54" s="257"/>
-      <c r="E54" s="258"/>
+      <c r="D54" s="270"/>
+      <c r="E54" s="271"/>
       <c r="F54" s="167" t="s">
         <v>71</v>
       </c>
@@ -7606,17 +7608,17 @@
       <c r="O54" s="78"/>
     </row>
     <row r="55" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="250">
+      <c r="A55" s="263">
         <v>29</v>
       </c>
       <c r="B55" s="198" t="s">
         <v>152</v>
       </c>
-      <c r="C55" s="256" t="s">
+      <c r="C55" s="269" t="s">
         <v>147</v>
       </c>
-      <c r="D55" s="257"/>
-      <c r="E55" s="258"/>
+      <c r="D55" s="270"/>
+      <c r="E55" s="271"/>
       <c r="F55" s="167" t="s">
         <v>71</v>
       </c>
@@ -7647,15 +7649,15 @@
       <c r="O55" s="78"/>
     </row>
     <row r="56" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="252"/>
+      <c r="A56" s="265"/>
       <c r="B56" s="198" t="s">
         <v>153</v>
       </c>
-      <c r="C56" s="256" t="s">
+      <c r="C56" s="269" t="s">
         <v>149</v>
       </c>
-      <c r="D56" s="257"/>
-      <c r="E56" s="258"/>
+      <c r="D56" s="270"/>
+      <c r="E56" s="271"/>
       <c r="F56" s="167" t="s">
         <v>71</v>
       </c>
@@ -7684,17 +7686,17 @@
       <c r="O56" s="78"/>
     </row>
     <row r="57" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="250">
+      <c r="A57" s="263">
         <v>30</v>
       </c>
       <c r="B57" s="198" t="s">
         <v>154</v>
       </c>
-      <c r="C57" s="256" t="s">
+      <c r="C57" s="269" t="s">
         <v>147</v>
       </c>
-      <c r="D57" s="257"/>
-      <c r="E57" s="258"/>
+      <c r="D57" s="270"/>
+      <c r="E57" s="271"/>
       <c r="F57" s="167" t="s">
         <v>71</v>
       </c>
@@ -7725,15 +7727,15 @@
       <c r="O57" s="78"/>
     </row>
     <row r="58" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="252"/>
+      <c r="A58" s="265"/>
       <c r="B58" s="198" t="s">
         <v>155</v>
       </c>
-      <c r="C58" s="256" t="s">
+      <c r="C58" s="269" t="s">
         <v>149</v>
       </c>
-      <c r="D58" s="257"/>
-      <c r="E58" s="258"/>
+      <c r="D58" s="270"/>
+      <c r="E58" s="271"/>
       <c r="F58" s="167" t="s">
         <v>71</v>
       </c>
@@ -7762,17 +7764,17 @@
       <c r="O58" s="78"/>
     </row>
     <row r="59" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="250">
+      <c r="A59" s="263">
         <v>31</v>
       </c>
       <c r="B59" s="156" t="s">
         <v>156</v>
       </c>
-      <c r="C59" s="256" t="s">
+      <c r="C59" s="269" t="s">
         <v>42</v>
       </c>
-      <c r="D59" s="257"/>
-      <c r="E59" s="258"/>
+      <c r="D59" s="270"/>
+      <c r="E59" s="271"/>
       <c r="F59" s="167" t="s">
         <v>71</v>
       </c>
@@ -7803,15 +7805,15 @@
       <c r="O59" s="78"/>
     </row>
     <row r="60" spans="1:15" s="79" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="252"/>
+      <c r="A60" s="265"/>
       <c r="B60" s="198" t="s">
         <v>158</v>
       </c>
-      <c r="C60" s="256" t="s">
+      <c r="C60" s="269" t="s">
         <v>54</v>
       </c>
-      <c r="D60" s="257"/>
-      <c r="E60" s="258"/>
+      <c r="D60" s="270"/>
+      <c r="E60" s="271"/>
       <c r="F60" s="167" t="s">
         <v>71</v>
       </c>
@@ -7839,17 +7841,17 @@
       <c r="N60" s="136"/>
     </row>
     <row r="61" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="250">
+      <c r="A61" s="263">
         <v>32</v>
       </c>
       <c r="B61" s="198" t="s">
         <v>159</v>
       </c>
-      <c r="C61" s="256" t="s">
+      <c r="C61" s="269" t="s">
         <v>160</v>
       </c>
-      <c r="D61" s="257"/>
-      <c r="E61" s="258"/>
+      <c r="D61" s="270"/>
+      <c r="E61" s="271"/>
       <c r="F61" s="167" t="s">
         <v>71</v>
       </c>
@@ -7880,15 +7882,15 @@
       <c r="O61" s="78"/>
     </row>
     <row r="62" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="252"/>
+      <c r="A62" s="265"/>
       <c r="B62" s="198" t="s">
         <v>161</v>
       </c>
-      <c r="C62" s="256" t="s">
+      <c r="C62" s="269" t="s">
         <v>162</v>
       </c>
-      <c r="D62" s="257"/>
-      <c r="E62" s="258"/>
+      <c r="D62" s="270"/>
+      <c r="E62" s="271"/>
       <c r="F62" s="167" t="s">
         <v>71</v>
       </c>
@@ -7923,11 +7925,11 @@
       <c r="B63" s="198" t="s">
         <v>163</v>
       </c>
-      <c r="C63" s="256" t="s">
+      <c r="C63" s="269" t="s">
         <v>164</v>
       </c>
-      <c r="D63" s="257"/>
-      <c r="E63" s="258"/>
+      <c r="D63" s="270"/>
+      <c r="E63" s="271"/>
       <c r="F63" s="167" t="s">
         <v>71</v>
       </c>
@@ -7964,11 +7966,11 @@
       <c r="B64" s="198" t="s">
         <v>167</v>
       </c>
-      <c r="C64" s="256" t="s">
+      <c r="C64" s="269" t="s">
         <v>164</v>
       </c>
-      <c r="D64" s="257"/>
-      <c r="E64" s="258"/>
+      <c r="D64" s="270"/>
+      <c r="E64" s="271"/>
       <c r="F64" s="167" t="s">
         <v>71</v>
       </c>
@@ -7999,17 +8001,17 @@
       <c r="O64" s="78"/>
     </row>
     <row r="65" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="250">
+      <c r="A65" s="263">
         <v>35</v>
       </c>
-      <c r="B65" s="272" t="s">
+      <c r="B65" s="307" t="s">
         <v>168</v>
       </c>
-      <c r="C65" s="256" t="s">
+      <c r="C65" s="269" t="s">
         <v>169</v>
       </c>
-      <c r="D65" s="257"/>
-      <c r="E65" s="258"/>
+      <c r="D65" s="270"/>
+      <c r="E65" s="271"/>
       <c r="F65" s="167" t="s">
         <v>71</v>
       </c>
@@ -8034,19 +8036,19 @@
       <c r="M65" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N65" s="248" t="s">
+      <c r="N65" s="317" t="s">
         <v>48</v>
       </c>
       <c r="O65" s="78"/>
     </row>
     <row r="66" spans="1:15" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="251"/>
-      <c r="B66" s="273"/>
-      <c r="C66" s="256" t="s">
+      <c r="A66" s="264"/>
+      <c r="B66" s="308"/>
+      <c r="C66" s="269" t="s">
         <v>60</v>
       </c>
-      <c r="D66" s="257"/>
-      <c r="E66" s="258"/>
+      <c r="D66" s="270"/>
+      <c r="E66" s="271"/>
       <c r="F66" s="167" t="s">
         <v>65</v>
       </c>
@@ -8071,16 +8073,16 @@
       <c r="M66" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N66" s="249"/>
+      <c r="N66" s="318"/>
     </row>
     <row r="67" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="252"/>
-      <c r="B67" s="274"/>
-      <c r="C67" s="256" t="s">
+      <c r="A67" s="265"/>
+      <c r="B67" s="309"/>
+      <c r="C67" s="269" t="s">
         <v>61</v>
       </c>
-      <c r="D67" s="257"/>
-      <c r="E67" s="258"/>
+      <c r="D67" s="270"/>
+      <c r="E67" s="271"/>
       <c r="F67" s="167" t="s">
         <v>65</v>
       </c>
@@ -8115,11 +8117,11 @@
       <c r="B68" s="162" t="s">
         <v>171</v>
       </c>
-      <c r="C68" s="256" t="s">
+      <c r="C68" s="269" t="s">
         <v>44</v>
       </c>
-      <c r="D68" s="257"/>
-      <c r="E68" s="258"/>
+      <c r="D68" s="270"/>
+      <c r="E68" s="271"/>
       <c r="F68" s="167" t="s">
         <v>71</v>
       </c>
@@ -8156,11 +8158,11 @@
       <c r="B69" s="162" t="s">
         <v>173</v>
       </c>
-      <c r="C69" s="256" t="s">
+      <c r="C69" s="269" t="s">
         <v>251</v>
       </c>
-      <c r="D69" s="257"/>
-      <c r="E69" s="258"/>
+      <c r="D69" s="270"/>
+      <c r="E69" s="271"/>
       <c r="F69" s="167" t="s">
         <v>71</v>
       </c>
@@ -8190,17 +8192,17 @@
       </c>
     </row>
     <row r="70" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="250">
+      <c r="A70" s="263">
         <v>38</v>
       </c>
       <c r="B70" s="156" t="s">
         <v>174</v>
       </c>
-      <c r="C70" s="256" t="s">
+      <c r="C70" s="269" t="s">
         <v>43</v>
       </c>
-      <c r="D70" s="257"/>
-      <c r="E70" s="258"/>
+      <c r="D70" s="270"/>
+      <c r="E70" s="271"/>
       <c r="F70" s="167" t="s">
         <v>71</v>
       </c>
@@ -8225,21 +8227,21 @@
       <c r="M70" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N70" s="248" t="s">
+      <c r="N70" s="317" t="s">
         <v>45</v>
       </c>
       <c r="O70" s="78"/>
     </row>
     <row r="71" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="252"/>
+      <c r="A71" s="265"/>
       <c r="B71" s="198" t="s">
         <v>175</v>
       </c>
-      <c r="C71" s="256" t="s">
+      <c r="C71" s="269" t="s">
         <v>55</v>
       </c>
-      <c r="D71" s="257"/>
-      <c r="E71" s="258"/>
+      <c r="D71" s="270"/>
+      <c r="E71" s="271"/>
       <c r="F71" s="167" t="s">
         <v>71</v>
       </c>
@@ -8264,21 +8266,21 @@
       <c r="M71" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N71" s="249"/>
+      <c r="N71" s="318"/>
       <c r="O71" s="78"/>
     </row>
     <row r="72" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="250">
+      <c r="A72" s="263">
         <v>39</v>
       </c>
       <c r="B72" s="198" t="s">
         <v>176</v>
       </c>
-      <c r="C72" s="256" t="s">
+      <c r="C72" s="269" t="s">
         <v>204</v>
       </c>
-      <c r="D72" s="257"/>
-      <c r="E72" s="258"/>
+      <c r="D72" s="270"/>
+      <c r="E72" s="271"/>
       <c r="F72" s="167" t="s">
         <v>71</v>
       </c>
@@ -8303,21 +8305,21 @@
       <c r="M72" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N72" s="248" t="s">
+      <c r="N72" s="317" t="s">
         <v>177</v>
       </c>
       <c r="O72" s="78"/>
     </row>
     <row r="73" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="252"/>
+      <c r="A73" s="265"/>
       <c r="B73" s="198" t="s">
         <v>178</v>
       </c>
-      <c r="C73" s="256" t="s">
+      <c r="C73" s="269" t="s">
         <v>205</v>
       </c>
-      <c r="D73" s="257"/>
-      <c r="E73" s="258"/>
+      <c r="D73" s="270"/>
+      <c r="E73" s="271"/>
       <c r="F73" s="167" t="s">
         <v>71</v>
       </c>
@@ -8342,7 +8344,7 @@
       <c r="M73" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N73" s="249"/>
+      <c r="N73" s="318"/>
       <c r="O73" s="78"/>
     </row>
     <row r="74" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8352,11 +8354,11 @@
       <c r="B74" s="198" t="s">
         <v>214</v>
       </c>
-      <c r="C74" s="256" t="s">
+      <c r="C74" s="269" t="s">
         <v>64</v>
       </c>
-      <c r="D74" s="257"/>
-      <c r="E74" s="258"/>
+      <c r="D74" s="270"/>
+      <c r="E74" s="271"/>
       <c r="F74" s="167" t="s">
         <v>71</v>
       </c>
@@ -8393,11 +8395,11 @@
       <c r="B75" s="198" t="s">
         <v>215</v>
       </c>
-      <c r="C75" s="256" t="s">
+      <c r="C75" s="269" t="s">
         <v>64</v>
       </c>
-      <c r="D75" s="257"/>
-      <c r="E75" s="258"/>
+      <c r="D75" s="270"/>
+      <c r="E75" s="271"/>
       <c r="F75" s="167" t="s">
         <v>71</v>
       </c>
@@ -8434,11 +8436,11 @@
       <c r="B76" s="198" t="s">
         <v>179</v>
       </c>
-      <c r="C76" s="256" t="s">
+      <c r="C76" s="269" t="s">
         <v>180</v>
       </c>
-      <c r="D76" s="257"/>
-      <c r="E76" s="258"/>
+      <c r="D76" s="270"/>
+      <c r="E76" s="271"/>
       <c r="F76" s="167" t="s">
         <v>71</v>
       </c>
@@ -8475,11 +8477,11 @@
       <c r="B77" s="198" t="s">
         <v>181</v>
       </c>
-      <c r="C77" s="256" t="s">
+      <c r="C77" s="269" t="s">
         <v>180</v>
       </c>
-      <c r="D77" s="257"/>
-      <c r="E77" s="258"/>
+      <c r="D77" s="270"/>
+      <c r="E77" s="271"/>
       <c r="F77" s="167" t="s">
         <v>71</v>
       </c>
@@ -8515,11 +8517,11 @@
       <c r="B78" s="198" t="s">
         <v>182</v>
       </c>
-      <c r="C78" s="256" t="s">
+      <c r="C78" s="269" t="s">
         <v>41</v>
       </c>
-      <c r="D78" s="257"/>
-      <c r="E78" s="258"/>
+      <c r="D78" s="270"/>
+      <c r="E78" s="271"/>
       <c r="F78" s="167" t="s">
         <v>71</v>
       </c>
@@ -8544,7 +8546,7 @@
       <c r="M78" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N78" s="248" t="s">
+      <c r="N78" s="317" t="s">
         <v>177</v>
       </c>
       <c r="O78" s="78"/>
@@ -8556,11 +8558,11 @@
       <c r="B79" s="198" t="s">
         <v>183</v>
       </c>
-      <c r="C79" s="256" t="s">
+      <c r="C79" s="269" t="s">
         <v>41</v>
       </c>
-      <c r="D79" s="257"/>
-      <c r="E79" s="258"/>
+      <c r="D79" s="270"/>
+      <c r="E79" s="271"/>
       <c r="F79" s="167" t="s">
         <v>71</v>
       </c>
@@ -8585,7 +8587,7 @@
       <c r="M79" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N79" s="249"/>
+      <c r="N79" s="318"/>
       <c r="O79" s="78"/>
     </row>
     <row r="80" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8595,11 +8597,11 @@
       <c r="B80" s="198" t="s">
         <v>184</v>
       </c>
-      <c r="C80" s="256" t="s">
+      <c r="C80" s="269" t="s">
         <v>53</v>
       </c>
-      <c r="D80" s="257"/>
-      <c r="E80" s="258"/>
+      <c r="D80" s="270"/>
+      <c r="E80" s="271"/>
       <c r="F80" s="167" t="s">
         <v>71</v>
       </c>
@@ -8634,11 +8636,11 @@
       <c r="B81" s="198" t="s">
         <v>185</v>
       </c>
-      <c r="C81" s="256" t="s">
+      <c r="C81" s="269" t="s">
         <v>53</v>
       </c>
-      <c r="D81" s="257"/>
-      <c r="E81" s="258"/>
+      <c r="D81" s="270"/>
+      <c r="E81" s="271"/>
       <c r="F81" s="167" t="s">
         <v>71</v>
       </c>
@@ -8673,11 +8675,11 @@
       <c r="B82" s="198" t="s">
         <v>186</v>
       </c>
-      <c r="C82" s="256" t="s">
+      <c r="C82" s="269" t="s">
         <v>187</v>
       </c>
-      <c r="D82" s="257"/>
-      <c r="E82" s="258"/>
+      <c r="D82" s="270"/>
+      <c r="E82" s="271"/>
       <c r="F82" s="167" t="s">
         <v>71</v>
       </c>
@@ -8702,7 +8704,7 @@
       <c r="M82" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N82" s="248" t="s">
+      <c r="N82" s="317" t="s">
         <v>177</v>
       </c>
       <c r="O82" s="78"/>
@@ -8714,11 +8716,11 @@
       <c r="B83" s="198" t="s">
         <v>188</v>
       </c>
-      <c r="C83" s="256" t="s">
+      <c r="C83" s="269" t="s">
         <v>187</v>
       </c>
-      <c r="D83" s="257"/>
-      <c r="E83" s="258"/>
+      <c r="D83" s="270"/>
+      <c r="E83" s="271"/>
       <c r="F83" s="167" t="s">
         <v>71</v>
       </c>
@@ -8743,7 +8745,7 @@
       <c r="M83" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N83" s="249"/>
+      <c r="N83" s="318"/>
       <c r="O83" s="78"/>
     </row>
     <row r="84" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8753,11 +8755,11 @@
       <c r="B84" s="198" t="s">
         <v>189</v>
       </c>
-      <c r="C84" s="256" t="s">
+      <c r="C84" s="269" t="s">
         <v>190</v>
       </c>
-      <c r="D84" s="257"/>
-      <c r="E84" s="258"/>
+      <c r="D84" s="270"/>
+      <c r="E84" s="271"/>
       <c r="F84" s="167" t="s">
         <v>71</v>
       </c>
@@ -8792,11 +8794,11 @@
       <c r="B85" s="198" t="s">
         <v>191</v>
       </c>
-      <c r="C85" s="256" t="s">
+      <c r="C85" s="269" t="s">
         <v>190</v>
       </c>
-      <c r="D85" s="257"/>
-      <c r="E85" s="258"/>
+      <c r="D85" s="270"/>
+      <c r="E85" s="271"/>
       <c r="F85" s="167" t="s">
         <v>71</v>
       </c>
@@ -8831,11 +8833,11 @@
       <c r="B86" s="158" t="s">
         <v>192</v>
       </c>
-      <c r="C86" s="256" t="s">
+      <c r="C86" s="269" t="s">
         <v>193</v>
       </c>
-      <c r="D86" s="257"/>
-      <c r="E86" s="258"/>
+      <c r="D86" s="270"/>
+      <c r="E86" s="271"/>
       <c r="F86" s="167" t="s">
         <v>71</v>
       </c>
@@ -8872,11 +8874,11 @@
       <c r="B87" s="198" t="s">
         <v>286</v>
       </c>
-      <c r="C87" s="259" t="s">
+      <c r="C87" s="266" t="s">
         <v>50</v>
       </c>
-      <c r="D87" s="260"/>
-      <c r="E87" s="261"/>
+      <c r="D87" s="267"/>
+      <c r="E87" s="268"/>
       <c r="F87" s="167" t="s">
         <v>71</v>
       </c>
@@ -8913,11 +8915,11 @@
       <c r="B88" s="167" t="s">
         <v>287</v>
       </c>
-      <c r="C88" s="259" t="s">
+      <c r="C88" s="266" t="s">
         <v>51</v>
       </c>
-      <c r="D88" s="260"/>
-      <c r="E88" s="261"/>
+      <c r="D88" s="267"/>
+      <c r="E88" s="268"/>
       <c r="F88" s="167" t="s">
         <v>71</v>
       </c>
@@ -8947,17 +8949,17 @@
       </c>
     </row>
     <row r="89" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="250">
+      <c r="A89" s="263">
         <v>55</v>
       </c>
-      <c r="B89" s="253" t="s">
+      <c r="B89" s="297" t="s">
         <v>283</v>
       </c>
-      <c r="C89" s="259" t="s">
+      <c r="C89" s="266" t="s">
         <v>78</v>
       </c>
-      <c r="D89" s="260"/>
-      <c r="E89" s="261"/>
+      <c r="D89" s="267"/>
+      <c r="E89" s="268"/>
       <c r="F89" s="167" t="s">
         <v>79</v>
       </c>
@@ -8986,13 +8988,13 @@
       <c r="O89" s="78"/>
     </row>
     <row r="90" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="251"/>
-      <c r="B90" s="254"/>
-      <c r="C90" s="259" t="s">
+      <c r="A90" s="264"/>
+      <c r="B90" s="298"/>
+      <c r="C90" s="266" t="s">
         <v>217</v>
       </c>
-      <c r="D90" s="260"/>
-      <c r="E90" s="261"/>
+      <c r="D90" s="267"/>
+      <c r="E90" s="268"/>
       <c r="F90" s="167" t="s">
         <v>79</v>
       </c>
@@ -9023,13 +9025,13 @@
       <c r="O90" s="78"/>
     </row>
     <row r="91" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="251"/>
-      <c r="B91" s="254"/>
-      <c r="C91" s="259" t="s">
+      <c r="A91" s="264"/>
+      <c r="B91" s="298"/>
+      <c r="C91" s="266" t="s">
         <v>218</v>
       </c>
-      <c r="D91" s="260"/>
-      <c r="E91" s="261"/>
+      <c r="D91" s="267"/>
+      <c r="E91" s="268"/>
       <c r="F91" s="167" t="s">
         <v>79</v>
       </c>
@@ -9060,13 +9062,13 @@
       <c r="O91" s="78"/>
     </row>
     <row r="92" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="251"/>
-      <c r="B92" s="254"/>
-      <c r="C92" s="259" t="s">
+      <c r="A92" s="264"/>
+      <c r="B92" s="298"/>
+      <c r="C92" s="266" t="s">
         <v>236</v>
       </c>
-      <c r="D92" s="260"/>
-      <c r="E92" s="261"/>
+      <c r="D92" s="267"/>
+      <c r="E92" s="268"/>
       <c r="F92" s="167" t="s">
         <v>79</v>
       </c>
@@ -9097,13 +9099,13 @@
       <c r="O92" s="78"/>
     </row>
     <row r="93" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="251"/>
-      <c r="B93" s="254"/>
-      <c r="C93" s="259" t="s">
+      <c r="A93" s="264"/>
+      <c r="B93" s="298"/>
+      <c r="C93" s="266" t="s">
         <v>237</v>
       </c>
-      <c r="D93" s="260"/>
-      <c r="E93" s="261"/>
+      <c r="D93" s="267"/>
+      <c r="E93" s="268"/>
       <c r="F93" s="167" t="s">
         <v>79</v>
       </c>
@@ -9134,13 +9136,13 @@
       <c r="O93" s="78"/>
     </row>
     <row r="94" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="251"/>
-      <c r="B94" s="254"/>
-      <c r="C94" s="259" t="s">
+      <c r="A94" s="264"/>
+      <c r="B94" s="298"/>
+      <c r="C94" s="266" t="s">
         <v>220</v>
       </c>
-      <c r="D94" s="260"/>
-      <c r="E94" s="261"/>
+      <c r="D94" s="267"/>
+      <c r="E94" s="268"/>
       <c r="F94" s="167" t="s">
         <v>79</v>
       </c>
@@ -9171,13 +9173,13 @@
       <c r="O94" s="78"/>
     </row>
     <row r="95" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="251"/>
-      <c r="B95" s="254"/>
-      <c r="C95" s="259" t="s">
+      <c r="A95" s="264"/>
+      <c r="B95" s="298"/>
+      <c r="C95" s="266" t="s">
         <v>221</v>
       </c>
-      <c r="D95" s="260"/>
-      <c r="E95" s="261"/>
+      <c r="D95" s="267"/>
+      <c r="E95" s="268"/>
       <c r="F95" s="167" t="s">
         <v>79</v>
       </c>
@@ -9208,13 +9210,13 @@
       <c r="O95" s="78"/>
     </row>
     <row r="96" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="251"/>
-      <c r="B96" s="254"/>
-      <c r="C96" s="259" t="s">
+      <c r="A96" s="264"/>
+      <c r="B96" s="298"/>
+      <c r="C96" s="266" t="s">
         <v>222</v>
       </c>
-      <c r="D96" s="260"/>
-      <c r="E96" s="261"/>
+      <c r="D96" s="267"/>
+      <c r="E96" s="268"/>
       <c r="F96" s="167" t="s">
         <v>79</v>
       </c>
@@ -9245,13 +9247,13 @@
       <c r="O96" s="78"/>
     </row>
     <row r="97" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="251"/>
-      <c r="B97" s="254"/>
-      <c r="C97" s="259" t="s">
+      <c r="A97" s="264"/>
+      <c r="B97" s="298"/>
+      <c r="C97" s="266" t="s">
         <v>223</v>
       </c>
-      <c r="D97" s="260"/>
-      <c r="E97" s="261"/>
+      <c r="D97" s="267"/>
+      <c r="E97" s="268"/>
       <c r="F97" s="167" t="s">
         <v>79</v>
       </c>
@@ -9282,13 +9284,13 @@
       <c r="O97" s="78"/>
     </row>
     <row r="98" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="251"/>
-      <c r="B98" s="254"/>
-      <c r="C98" s="259" t="s">
+      <c r="A98" s="264"/>
+      <c r="B98" s="298"/>
+      <c r="C98" s="266" t="s">
         <v>224</v>
       </c>
-      <c r="D98" s="260"/>
-      <c r="E98" s="261"/>
+      <c r="D98" s="267"/>
+      <c r="E98" s="268"/>
       <c r="F98" s="167" t="s">
         <v>79</v>
       </c>
@@ -9319,13 +9321,13 @@
       <c r="O98" s="78"/>
     </row>
     <row r="99" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="251"/>
-      <c r="B99" s="254"/>
-      <c r="C99" s="259" t="s">
+      <c r="A99" s="264"/>
+      <c r="B99" s="298"/>
+      <c r="C99" s="266" t="s">
         <v>225</v>
       </c>
-      <c r="D99" s="260"/>
-      <c r="E99" s="261"/>
+      <c r="D99" s="267"/>
+      <c r="E99" s="268"/>
       <c r="F99" s="167" t="s">
         <v>79</v>
       </c>
@@ -9356,13 +9358,13 @@
       <c r="O99" s="78"/>
     </row>
     <row r="100" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="251"/>
-      <c r="B100" s="254"/>
-      <c r="C100" s="259" t="s">
+      <c r="A100" s="264"/>
+      <c r="B100" s="298"/>
+      <c r="C100" s="266" t="s">
         <v>226</v>
       </c>
-      <c r="D100" s="260"/>
-      <c r="E100" s="261"/>
+      <c r="D100" s="267"/>
+      <c r="E100" s="268"/>
       <c r="F100" s="167" t="s">
         <v>79</v>
       </c>
@@ -9393,13 +9395,13 @@
       <c r="O100" s="78"/>
     </row>
     <row r="101" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="251"/>
-      <c r="B101" s="254"/>
-      <c r="C101" s="259" t="s">
+      <c r="A101" s="264"/>
+      <c r="B101" s="298"/>
+      <c r="C101" s="266" t="s">
         <v>260</v>
       </c>
-      <c r="D101" s="260"/>
-      <c r="E101" s="261"/>
+      <c r="D101" s="267"/>
+      <c r="E101" s="268"/>
       <c r="F101" s="167" t="s">
         <v>79</v>
       </c>
@@ -9430,13 +9432,13 @@
       <c r="O101" s="78"/>
     </row>
     <row r="102" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="251"/>
-      <c r="B102" s="254"/>
-      <c r="C102" s="259" t="s">
+      <c r="A102" s="264"/>
+      <c r="B102" s="298"/>
+      <c r="C102" s="266" t="s">
         <v>227</v>
       </c>
-      <c r="D102" s="260"/>
-      <c r="E102" s="261"/>
+      <c r="D102" s="267"/>
+      <c r="E102" s="268"/>
       <c r="F102" s="167" t="s">
         <v>79</v>
       </c>
@@ -9467,13 +9469,13 @@
       <c r="O102" s="78"/>
     </row>
     <row r="103" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="251"/>
-      <c r="B103" s="254"/>
-      <c r="C103" s="259" t="s">
+      <c r="A103" s="264"/>
+      <c r="B103" s="298"/>
+      <c r="C103" s="266" t="s">
         <v>228</v>
       </c>
-      <c r="D103" s="260"/>
-      <c r="E103" s="261"/>
+      <c r="D103" s="267"/>
+      <c r="E103" s="268"/>
       <c r="F103" s="167" t="s">
         <v>79</v>
       </c>
@@ -9504,13 +9506,13 @@
       <c r="O103" s="78"/>
     </row>
     <row r="104" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="251"/>
-      <c r="B104" s="254"/>
-      <c r="C104" s="259" t="s">
+      <c r="A104" s="264"/>
+      <c r="B104" s="298"/>
+      <c r="C104" s="266" t="s">
         <v>44</v>
       </c>
-      <c r="D104" s="260"/>
-      <c r="E104" s="261"/>
+      <c r="D104" s="267"/>
+      <c r="E104" s="268"/>
       <c r="F104" s="167" t="s">
         <v>79</v>
       </c>
@@ -9541,13 +9543,13 @@
       <c r="O104" s="78"/>
     </row>
     <row r="105" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="251"/>
-      <c r="B105" s="254"/>
-      <c r="C105" s="259" t="s">
+      <c r="A105" s="264"/>
+      <c r="B105" s="298"/>
+      <c r="C105" s="266" t="s">
         <v>229</v>
       </c>
-      <c r="D105" s="260"/>
-      <c r="E105" s="261"/>
+      <c r="D105" s="267"/>
+      <c r="E105" s="268"/>
       <c r="F105" s="167" t="s">
         <v>79</v>
       </c>
@@ -9578,13 +9580,13 @@
       <c r="O105" s="78"/>
     </row>
     <row r="106" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="251"/>
-      <c r="B106" s="254"/>
-      <c r="C106" s="259" t="s">
+      <c r="A106" s="264"/>
+      <c r="B106" s="298"/>
+      <c r="C106" s="266" t="s">
         <v>238</v>
       </c>
-      <c r="D106" s="260"/>
-      <c r="E106" s="261"/>
+      <c r="D106" s="267"/>
+      <c r="E106" s="268"/>
       <c r="F106" s="167" t="s">
         <v>79</v>
       </c>
@@ -9615,13 +9617,13 @@
       <c r="O106" s="78"/>
     </row>
     <row r="107" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="251"/>
-      <c r="B107" s="254"/>
-      <c r="C107" s="259" t="s">
+      <c r="A107" s="264"/>
+      <c r="B107" s="298"/>
+      <c r="C107" s="266" t="s">
         <v>230</v>
       </c>
-      <c r="D107" s="260"/>
-      <c r="E107" s="261"/>
+      <c r="D107" s="267"/>
+      <c r="E107" s="268"/>
       <c r="F107" s="167" t="s">
         <v>79</v>
       </c>
@@ -9652,13 +9654,13 @@
       <c r="O107" s="78"/>
     </row>
     <row r="108" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="251"/>
-      <c r="B108" s="254"/>
-      <c r="C108" s="259" t="s">
+      <c r="A108" s="264"/>
+      <c r="B108" s="298"/>
+      <c r="C108" s="266" t="s">
         <v>230</v>
       </c>
-      <c r="D108" s="260"/>
-      <c r="E108" s="261"/>
+      <c r="D108" s="267"/>
+      <c r="E108" s="268"/>
       <c r="F108" s="167" t="s">
         <v>79</v>
       </c>
@@ -9689,13 +9691,13 @@
       <c r="O108" s="78"/>
     </row>
     <row r="109" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="251"/>
-      <c r="B109" s="254"/>
-      <c r="C109" s="259" t="s">
+      <c r="A109" s="264"/>
+      <c r="B109" s="298"/>
+      <c r="C109" s="266" t="s">
         <v>230</v>
       </c>
-      <c r="D109" s="260"/>
-      <c r="E109" s="261"/>
+      <c r="D109" s="267"/>
+      <c r="E109" s="268"/>
       <c r="F109" s="167" t="s">
         <v>79</v>
       </c>
@@ -9726,13 +9728,13 @@
       <c r="O109" s="78"/>
     </row>
     <row r="110" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="251"/>
-      <c r="B110" s="254"/>
-      <c r="C110" s="259" t="s">
+      <c r="A110" s="264"/>
+      <c r="B110" s="298"/>
+      <c r="C110" s="266" t="s">
         <v>231</v>
       </c>
-      <c r="D110" s="260"/>
-      <c r="E110" s="261"/>
+      <c r="D110" s="267"/>
+      <c r="E110" s="268"/>
       <c r="F110" s="167" t="s">
         <v>79</v>
       </c>
@@ -9763,13 +9765,13 @@
       <c r="O110" s="78"/>
     </row>
     <row r="111" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="251"/>
-      <c r="B111" s="254"/>
-      <c r="C111" s="259" t="s">
+      <c r="A111" s="264"/>
+      <c r="B111" s="298"/>
+      <c r="C111" s="266" t="s">
         <v>248</v>
       </c>
-      <c r="D111" s="260"/>
-      <c r="E111" s="261"/>
+      <c r="D111" s="267"/>
+      <c r="E111" s="268"/>
       <c r="F111" s="167" t="s">
         <v>79</v>
       </c>
@@ -9800,13 +9802,13 @@
       <c r="O111" s="78"/>
     </row>
     <row r="112" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="251"/>
-      <c r="B112" s="254"/>
-      <c r="C112" s="259" t="s">
+      <c r="A112" s="264"/>
+      <c r="B112" s="298"/>
+      <c r="C112" s="266" t="s">
         <v>261</v>
       </c>
-      <c r="D112" s="260"/>
-      <c r="E112" s="261"/>
+      <c r="D112" s="267"/>
+      <c r="E112" s="268"/>
       <c r="F112" s="163" t="s">
         <v>87</v>
       </c>
@@ -9837,13 +9839,13 @@
       <c r="O112" s="78"/>
     </row>
     <row r="113" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="251"/>
-      <c r="B113" s="254"/>
-      <c r="C113" s="259" t="s">
+      <c r="A113" s="264"/>
+      <c r="B113" s="298"/>
+      <c r="C113" s="266" t="s">
         <v>200</v>
       </c>
-      <c r="D113" s="260"/>
-      <c r="E113" s="261"/>
+      <c r="D113" s="267"/>
+      <c r="E113" s="268"/>
       <c r="F113" s="167" t="s">
         <v>78</v>
       </c>
@@ -9874,13 +9876,13 @@
       <c r="O113" s="78"/>
     </row>
     <row r="114" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="251"/>
-      <c r="B114" s="254"/>
-      <c r="C114" s="256" t="s">
+      <c r="A114" s="264"/>
+      <c r="B114" s="298"/>
+      <c r="C114" s="269" t="s">
         <v>194</v>
       </c>
-      <c r="D114" s="257"/>
-      <c r="E114" s="258"/>
+      <c r="D114" s="270"/>
+      <c r="E114" s="271"/>
       <c r="F114" s="167" t="s">
         <v>232</v>
       </c>
@@ -9911,13 +9913,13 @@
       <c r="O114" s="78"/>
     </row>
     <row r="115" spans="1:15" s="171" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="251"/>
-      <c r="B115" s="254"/>
-      <c r="C115" s="262" t="s">
+      <c r="A115" s="264"/>
+      <c r="B115" s="298"/>
+      <c r="C115" s="319" t="s">
         <v>263</v>
       </c>
-      <c r="D115" s="263"/>
-      <c r="E115" s="264"/>
+      <c r="D115" s="320"/>
+      <c r="E115" s="321"/>
       <c r="F115" s="203" t="s">
         <v>78</v>
       </c>
@@ -9947,13 +9949,13 @@
       </c>
     </row>
     <row r="116" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="252"/>
-      <c r="B116" s="255"/>
-      <c r="C116" s="259" t="s">
+      <c r="A116" s="265"/>
+      <c r="B116" s="299"/>
+      <c r="C116" s="266" t="s">
         <v>76</v>
       </c>
-      <c r="D116" s="260"/>
-      <c r="E116" s="261"/>
+      <c r="D116" s="267"/>
+      <c r="E116" s="268"/>
       <c r="F116" s="167" t="s">
         <v>263</v>
       </c>
@@ -9984,17 +9986,17 @@
       <c r="O116" s="78"/>
     </row>
     <row r="117" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="250">
+      <c r="A117" s="263">
         <v>56</v>
       </c>
-      <c r="B117" s="253" t="s">
+      <c r="B117" s="297" t="s">
         <v>284</v>
       </c>
-      <c r="C117" s="259" t="s">
+      <c r="C117" s="266" t="s">
         <v>66</v>
       </c>
-      <c r="D117" s="260"/>
-      <c r="E117" s="261"/>
+      <c r="D117" s="267"/>
+      <c r="E117" s="268"/>
       <c r="F117" s="167" t="s">
         <v>76</v>
       </c>
@@ -10025,13 +10027,13 @@
       <c r="O117" s="78"/>
     </row>
     <row r="118" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="251"/>
-      <c r="B118" s="254"/>
-      <c r="C118" s="259" t="s">
+      <c r="A118" s="264"/>
+      <c r="B118" s="298"/>
+      <c r="C118" s="266" t="s">
         <v>67</v>
       </c>
-      <c r="D118" s="260"/>
-      <c r="E118" s="261"/>
+      <c r="D118" s="267"/>
+      <c r="E118" s="268"/>
       <c r="F118" s="167" t="s">
         <v>76</v>
       </c>
@@ -10062,13 +10064,13 @@
       <c r="O118" s="78"/>
     </row>
     <row r="119" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="251"/>
-      <c r="B119" s="254"/>
-      <c r="C119" s="259" t="s">
+      <c r="A119" s="264"/>
+      <c r="B119" s="298"/>
+      <c r="C119" s="266" t="s">
         <v>68</v>
       </c>
-      <c r="D119" s="260"/>
-      <c r="E119" s="261"/>
+      <c r="D119" s="267"/>
+      <c r="E119" s="268"/>
       <c r="F119" s="167" t="s">
         <v>76</v>
       </c>
@@ -10099,13 +10101,13 @@
       <c r="O119" s="78"/>
     </row>
     <row r="120" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="252"/>
-      <c r="B120" s="255"/>
-      <c r="C120" s="259" t="s">
+      <c r="A120" s="265"/>
+      <c r="B120" s="299"/>
+      <c r="C120" s="266" t="s">
         <v>69</v>
       </c>
-      <c r="D120" s="260"/>
-      <c r="E120" s="261"/>
+      <c r="D120" s="267"/>
+      <c r="E120" s="268"/>
       <c r="F120" s="167" t="s">
         <v>76</v>
       </c>
@@ -10136,17 +10138,17 @@
       <c r="O120" s="78"/>
     </row>
     <row r="121" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="250">
+      <c r="A121" s="263">
         <v>57</v>
       </c>
-      <c r="B121" s="253" t="s">
+      <c r="B121" s="297" t="s">
         <v>285</v>
       </c>
-      <c r="C121" s="256" t="s">
+      <c r="C121" s="269" t="s">
         <v>85</v>
       </c>
-      <c r="D121" s="257"/>
-      <c r="E121" s="258"/>
+      <c r="D121" s="270"/>
+      <c r="E121" s="271"/>
       <c r="F121" s="167" t="s">
         <v>71</v>
       </c>
@@ -10177,13 +10179,13 @@
       <c r="O121" s="78"/>
     </row>
     <row r="122" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="251"/>
-      <c r="B122" s="254"/>
-      <c r="C122" s="256" t="s">
+      <c r="A122" s="264"/>
+      <c r="B122" s="298"/>
+      <c r="C122" s="269" t="s">
         <v>209</v>
       </c>
-      <c r="D122" s="257"/>
-      <c r="E122" s="258"/>
+      <c r="D122" s="270"/>
+      <c r="E122" s="271"/>
       <c r="F122" s="167" t="s">
         <v>73</v>
       </c>
@@ -10214,13 +10216,13 @@
       <c r="O122" s="78"/>
     </row>
     <row r="123" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="251"/>
-      <c r="B123" s="254"/>
-      <c r="C123" s="256" t="s">
+      <c r="A123" s="264"/>
+      <c r="B123" s="298"/>
+      <c r="C123" s="269" t="s">
         <v>210</v>
       </c>
-      <c r="D123" s="257"/>
-      <c r="E123" s="258"/>
+      <c r="D123" s="270"/>
+      <c r="E123" s="271"/>
       <c r="F123" s="167" t="s">
         <v>73</v>
       </c>
@@ -10251,13 +10253,13 @@
       <c r="O123" s="78"/>
     </row>
     <row r="124" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="251"/>
-      <c r="B124" s="254"/>
-      <c r="C124" s="256" t="s">
+      <c r="A124" s="264"/>
+      <c r="B124" s="298"/>
+      <c r="C124" s="269" t="s">
         <v>211</v>
       </c>
-      <c r="D124" s="257"/>
-      <c r="E124" s="258"/>
+      <c r="D124" s="270"/>
+      <c r="E124" s="271"/>
       <c r="F124" s="167" t="s">
         <v>73</v>
       </c>
@@ -10288,13 +10290,13 @@
       <c r="O124" s="78"/>
     </row>
     <row r="125" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="251"/>
-      <c r="B125" s="254"/>
-      <c r="C125" s="256" t="s">
+      <c r="A125" s="264"/>
+      <c r="B125" s="298"/>
+      <c r="C125" s="269" t="s">
         <v>62</v>
       </c>
-      <c r="D125" s="257"/>
-      <c r="E125" s="258"/>
+      <c r="D125" s="270"/>
+      <c r="E125" s="271"/>
       <c r="F125" s="167" t="s">
         <v>73</v>
       </c>
@@ -10325,13 +10327,13 @@
       <c r="O125" s="78"/>
     </row>
     <row r="126" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="251"/>
-      <c r="B126" s="254"/>
-      <c r="C126" s="256" t="s">
+      <c r="A126" s="264"/>
+      <c r="B126" s="298"/>
+      <c r="C126" s="269" t="s">
         <v>63</v>
       </c>
-      <c r="D126" s="257"/>
-      <c r="E126" s="258"/>
+      <c r="D126" s="270"/>
+      <c r="E126" s="271"/>
       <c r="F126" s="167" t="s">
         <v>73</v>
       </c>
@@ -10362,13 +10364,13 @@
       <c r="O126" s="78"/>
     </row>
     <row r="127" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="251"/>
-      <c r="B127" s="254"/>
-      <c r="C127" s="256" t="s">
+      <c r="A127" s="264"/>
+      <c r="B127" s="298"/>
+      <c r="C127" s="269" t="s">
         <v>197</v>
       </c>
-      <c r="D127" s="257"/>
-      <c r="E127" s="258"/>
+      <c r="D127" s="270"/>
+      <c r="E127" s="271"/>
       <c r="F127" s="167" t="s">
         <v>73</v>
       </c>
@@ -10399,13 +10401,13 @@
       <c r="O127" s="78"/>
     </row>
     <row r="128" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="251"/>
-      <c r="B128" s="254"/>
-      <c r="C128" s="256" t="s">
+      <c r="A128" s="264"/>
+      <c r="B128" s="298"/>
+      <c r="C128" s="269" t="s">
         <v>198</v>
       </c>
-      <c r="D128" s="257"/>
-      <c r="E128" s="258"/>
+      <c r="D128" s="270"/>
+      <c r="E128" s="271"/>
       <c r="F128" s="167" t="s">
         <v>73</v>
       </c>
@@ -10436,13 +10438,13 @@
       <c r="O128" s="78"/>
     </row>
     <row r="129" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="251"/>
-      <c r="B129" s="254"/>
-      <c r="C129" s="256" t="s">
+      <c r="A129" s="264"/>
+      <c r="B129" s="298"/>
+      <c r="C129" s="269" t="s">
         <v>208</v>
       </c>
-      <c r="D129" s="257"/>
-      <c r="E129" s="258"/>
+      <c r="D129" s="270"/>
+      <c r="E129" s="271"/>
       <c r="F129" s="167" t="s">
         <v>73</v>
       </c>
@@ -10473,13 +10475,13 @@
       <c r="O129" s="78"/>
     </row>
     <row r="130" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="251"/>
-      <c r="B130" s="254"/>
-      <c r="C130" s="256" t="s">
+      <c r="A130" s="264"/>
+      <c r="B130" s="298"/>
+      <c r="C130" s="269" t="s">
         <v>202</v>
       </c>
-      <c r="D130" s="257"/>
-      <c r="E130" s="258"/>
+      <c r="D130" s="270"/>
+      <c r="E130" s="271"/>
       <c r="F130" s="167" t="s">
         <v>73</v>
       </c>
@@ -10510,13 +10512,13 @@
       <c r="O130" s="78"/>
     </row>
     <row r="131" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="251"/>
-      <c r="B131" s="254"/>
-      <c r="C131" s="256" t="s">
+      <c r="A131" s="264"/>
+      <c r="B131" s="298"/>
+      <c r="C131" s="269" t="s">
         <v>264</v>
       </c>
-      <c r="D131" s="257"/>
-      <c r="E131" s="258"/>
+      <c r="D131" s="270"/>
+      <c r="E131" s="271"/>
       <c r="F131" s="167" t="s">
         <v>73</v>
       </c>
@@ -10547,13 +10549,13 @@
       <c r="O131" s="78"/>
     </row>
     <row r="132" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="251"/>
-      <c r="B132" s="254"/>
-      <c r="C132" s="256" t="s">
+      <c r="A132" s="264"/>
+      <c r="B132" s="298"/>
+      <c r="C132" s="269" t="s">
         <v>199</v>
       </c>
-      <c r="D132" s="257"/>
-      <c r="E132" s="258"/>
+      <c r="D132" s="270"/>
+      <c r="E132" s="271"/>
       <c r="F132" s="167" t="s">
         <v>73</v>
       </c>
@@ -10584,13 +10586,13 @@
       <c r="O132" s="78"/>
     </row>
     <row r="133" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="251"/>
-      <c r="B133" s="254"/>
-      <c r="C133" s="256" t="s">
+      <c r="A133" s="264"/>
+      <c r="B133" s="298"/>
+      <c r="C133" s="269" t="s">
         <v>212</v>
       </c>
-      <c r="D133" s="257"/>
-      <c r="E133" s="258"/>
+      <c r="D133" s="270"/>
+      <c r="E133" s="271"/>
       <c r="F133" s="167" t="s">
         <v>73</v>
       </c>
@@ -10621,13 +10623,13 @@
       <c r="O133" s="78"/>
     </row>
     <row r="134" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="252"/>
-      <c r="B134" s="255"/>
-      <c r="C134" s="256" t="s">
+      <c r="A134" s="265"/>
+      <c r="B134" s="299"/>
+      <c r="C134" s="269" t="s">
         <v>213</v>
       </c>
-      <c r="D134" s="257"/>
-      <c r="E134" s="258"/>
+      <c r="D134" s="270"/>
+      <c r="E134" s="271"/>
       <c r="F134" s="167" t="s">
         <v>73</v>
       </c>
@@ -10660,9 +10662,9 @@
     <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135" s="197"/>
       <c r="B135" s="144"/>
-      <c r="C135" s="297"/>
-      <c r="D135" s="298"/>
-      <c r="E135" s="299"/>
+      <c r="C135" s="300"/>
+      <c r="D135" s="301"/>
+      <c r="E135" s="302"/>
       <c r="F135" s="118"/>
       <c r="G135" s="119"/>
       <c r="H135" s="119"/>
@@ -10679,9 +10681,9 @@
       <c r="B136" s="200"/>
       <c r="C136" s="201"/>
       <c r="D136" s="202"/>
-      <c r="E136" s="285"/>
-      <c r="F136" s="286"/>
-      <c r="G136" s="287"/>
+      <c r="E136" s="288"/>
+      <c r="F136" s="289"/>
+      <c r="G136" s="290"/>
       <c r="H136" s="165"/>
       <c r="I136" s="165"/>
       <c r="J136" s="165"/>
@@ -10696,9 +10698,9 @@
       <c r="B137" s="200"/>
       <c r="C137" s="201"/>
       <c r="D137" s="202"/>
-      <c r="E137" s="288"/>
-      <c r="F137" s="289"/>
-      <c r="G137" s="290"/>
+      <c r="E137" s="291"/>
+      <c r="F137" s="292"/>
+      <c r="G137" s="293"/>
       <c r="H137" s="165"/>
       <c r="I137" s="165"/>
       <c r="J137" s="165"/>
@@ -10712,13 +10714,13 @@
       <c r="A138" s="94" t="s">
         <v>295</v>
       </c>
-      <c r="B138" s="291" t="s">
+      <c r="B138" s="322">
+        <v>42136</v>
+      </c>
+      <c r="C138" s="323"/>
+      <c r="D138" s="324"/>
+      <c r="E138" s="294" t="s">
         <v>296</v>
-      </c>
-      <c r="C138" s="292"/>
-      <c r="D138" s="293"/>
-      <c r="E138" s="294" t="s">
-        <v>297</v>
       </c>
       <c r="F138" s="295"/>
       <c r="G138" s="296"/>
@@ -10741,16 +10743,16 @@
       <c r="A139" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="B139" s="279" t="s">
+      <c r="B139" s="282" t="s">
         <v>33</v>
       </c>
-      <c r="C139" s="280"/>
-      <c r="D139" s="281"/>
-      <c r="E139" s="282" t="s">
+      <c r="C139" s="283"/>
+      <c r="D139" s="284"/>
+      <c r="E139" s="285" t="s">
         <v>36</v>
       </c>
-      <c r="F139" s="283"/>
-      <c r="G139" s="284"/>
+      <c r="F139" s="286"/>
+      <c r="G139" s="287"/>
       <c r="H139" s="164"/>
       <c r="I139" s="164"/>
       <c r="J139" s="164"/>
@@ -12059,6 +12061,161 @@
     </row>
   </sheetData>
   <mergeCells count="179">
+    <mergeCell ref="N72:N73"/>
+    <mergeCell ref="A121:A134"/>
+    <mergeCell ref="B121:B134"/>
+    <mergeCell ref="N70:N71"/>
+    <mergeCell ref="C133:E133"/>
+    <mergeCell ref="C134:E134"/>
+    <mergeCell ref="N82:N83"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="C86:E86"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="N78:N79"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="C131:E131"/>
+    <mergeCell ref="C128:E128"/>
+    <mergeCell ref="C111:E111"/>
+    <mergeCell ref="C115:E115"/>
+    <mergeCell ref="C108:E108"/>
+    <mergeCell ref="C107:E107"/>
+    <mergeCell ref="C129:E129"/>
+    <mergeCell ref="B89:B116"/>
+    <mergeCell ref="A89:A116"/>
+    <mergeCell ref="C99:E99"/>
+    <mergeCell ref="C100:E100"/>
+    <mergeCell ref="C101:E101"/>
+    <mergeCell ref="C109:E109"/>
+    <mergeCell ref="C110:E110"/>
+    <mergeCell ref="C102:E102"/>
+    <mergeCell ref="C103:E103"/>
+    <mergeCell ref="C104:E104"/>
+    <mergeCell ref="C105:E105"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="M6:N8"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="N65:N66"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="C94:E94"/>
+    <mergeCell ref="C77:E77"/>
+    <mergeCell ref="C87:E87"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="C93:E93"/>
+    <mergeCell ref="C82:E82"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="B139:D139"/>
+    <mergeCell ref="E139:G139"/>
+    <mergeCell ref="C97:E97"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="C122:E122"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C124:E124"/>
+    <mergeCell ref="C125:E125"/>
+    <mergeCell ref="C126:E126"/>
+    <mergeCell ref="C127:E127"/>
+    <mergeCell ref="E136:G136"/>
+    <mergeCell ref="E137:G137"/>
+    <mergeCell ref="B138:D138"/>
+    <mergeCell ref="E138:G138"/>
+    <mergeCell ref="C114:E114"/>
+    <mergeCell ref="B117:B120"/>
+    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="C118:E118"/>
+    <mergeCell ref="C119:E119"/>
+    <mergeCell ref="C120:E120"/>
+    <mergeCell ref="C135:E135"/>
+    <mergeCell ref="C130:E130"/>
+    <mergeCell ref="C132:E132"/>
+    <mergeCell ref="C98:E98"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="F1:G5"/>
     <mergeCell ref="D9:G9"/>
@@ -12083,164 +12240,9 @@
     <mergeCell ref="C41:E41"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="C47:E47"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="B139:D139"/>
-    <mergeCell ref="E139:G139"/>
-    <mergeCell ref="C97:E97"/>
-    <mergeCell ref="C121:E121"/>
-    <mergeCell ref="C122:E122"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C124:E124"/>
-    <mergeCell ref="C125:E125"/>
-    <mergeCell ref="C126:E126"/>
-    <mergeCell ref="C127:E127"/>
-    <mergeCell ref="E136:G136"/>
-    <mergeCell ref="E137:G137"/>
-    <mergeCell ref="B138:D138"/>
-    <mergeCell ref="E138:G138"/>
-    <mergeCell ref="C114:E114"/>
-    <mergeCell ref="B117:B120"/>
-    <mergeCell ref="C117:E117"/>
-    <mergeCell ref="C118:E118"/>
-    <mergeCell ref="C119:E119"/>
-    <mergeCell ref="C120:E120"/>
-    <mergeCell ref="C135:E135"/>
-    <mergeCell ref="C130:E130"/>
-    <mergeCell ref="C132:E132"/>
-    <mergeCell ref="C98:E98"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="C94:E94"/>
-    <mergeCell ref="C77:E77"/>
-    <mergeCell ref="C87:E87"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="C90:E90"/>
-    <mergeCell ref="C91:E91"/>
-    <mergeCell ref="C93:E93"/>
-    <mergeCell ref="C82:E82"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="M6:N8"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="N65:N66"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C115:E115"/>
-    <mergeCell ref="C108:E108"/>
-    <mergeCell ref="C107:E107"/>
-    <mergeCell ref="C129:E129"/>
-    <mergeCell ref="B89:B116"/>
-    <mergeCell ref="A89:A116"/>
-    <mergeCell ref="C99:E99"/>
-    <mergeCell ref="C100:E100"/>
-    <mergeCell ref="C101:E101"/>
-    <mergeCell ref="C109:E109"/>
-    <mergeCell ref="C110:E110"/>
-    <mergeCell ref="C102:E102"/>
-    <mergeCell ref="C103:E103"/>
-    <mergeCell ref="C104:E104"/>
-    <mergeCell ref="C105:E105"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="N72:N73"/>
-    <mergeCell ref="A121:A134"/>
-    <mergeCell ref="B121:B134"/>
-    <mergeCell ref="N70:N71"/>
-    <mergeCell ref="C133:E133"/>
-    <mergeCell ref="C134:E134"/>
-    <mergeCell ref="N82:N83"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C84:E84"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="C86:E86"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="N78:N79"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="C131:E131"/>
-    <mergeCell ref="C128:E128"/>
-    <mergeCell ref="C111:E111"/>
   </mergeCells>
-  <pageMargins left="1.5" right="0.25" top="0.5" bottom="0.25" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="90" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="1.5093749999999999" right="0.25" top="0.5" bottom="0.25" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" scale="55" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed .bak files and fixed page size of Cable Schedule
</commit_message>
<xml_diff>
--- a/Specification/240-0201-EMEL-CL00-0001 CABLE SCHEDULE/P-240 CABLE SCHEDULE 11.11.15.xlsx
+++ b/Specification/240-0201-EMEL-CL00-0001 CABLE SCHEDULE/P-240 CABLE SCHEDULE 11.11.15.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="COVER" sheetId="7" r:id="rId1"/>
@@ -102,7 +102,7 @@
     <definedName name="Y">#REF!</definedName>
     <definedName name="zq_syst">'[3]CASE A1 CPP'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1011,7 +1011,7 @@
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="General_)"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="168" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -2491,6 +2491,12 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="44" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="43" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="44" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2704,6 +2710,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2787,21 +2802,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="15" fillId="2" borderId="43" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="15" fillId="2" borderId="44" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -3086,8 +3086,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7814302" y="102144"/>
-          <a:ext cx="1015373" cy="726531"/>
+          <a:off x="7721773" y="102144"/>
+          <a:ext cx="994963" cy="737417"/>
           <a:chOff x="7337307" y="99264"/>
           <a:chExt cx="684810" cy="511264"/>
         </a:xfrm>
@@ -4551,7 +4551,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
@@ -4591,94 +4591,94 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="213"/>
-      <c r="C2" s="214"/>
-      <c r="D2" s="214"/>
-      <c r="E2" s="214"/>
-      <c r="F2" s="214"/>
-      <c r="G2" s="215"/>
-      <c r="H2" s="219" t="s">
+      <c r="B2" s="215"/>
+      <c r="C2" s="216"/>
+      <c r="D2" s="216"/>
+      <c r="E2" s="216"/>
+      <c r="F2" s="216"/>
+      <c r="G2" s="217"/>
+      <c r="H2" s="221" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="220"/>
-      <c r="J2" s="220"/>
-      <c r="K2" s="220"/>
-      <c r="L2" s="220"/>
-      <c r="M2" s="220"/>
-      <c r="N2" s="220"/>
-      <c r="O2" s="221"/>
+      <c r="I2" s="222"/>
+      <c r="J2" s="222"/>
+      <c r="K2" s="222"/>
+      <c r="L2" s="222"/>
+      <c r="M2" s="222"/>
+      <c r="N2" s="222"/>
+      <c r="O2" s="223"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="216"/>
-      <c r="C3" s="217"/>
-      <c r="D3" s="217"/>
-      <c r="E3" s="217"/>
-      <c r="F3" s="217"/>
-      <c r="G3" s="218"/>
-      <c r="H3" s="222" t="s">
+      <c r="B3" s="218"/>
+      <c r="C3" s="219"/>
+      <c r="D3" s="219"/>
+      <c r="E3" s="219"/>
+      <c r="F3" s="219"/>
+      <c r="G3" s="220"/>
+      <c r="H3" s="224" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="223"/>
-      <c r="J3" s="223"/>
-      <c r="K3" s="223"/>
-      <c r="L3" s="223"/>
-      <c r="M3" s="223"/>
-      <c r="N3" s="223"/>
-      <c r="O3" s="224"/>
+      <c r="I3" s="225"/>
+      <c r="J3" s="225"/>
+      <c r="K3" s="225"/>
+      <c r="L3" s="225"/>
+      <c r="M3" s="225"/>
+      <c r="N3" s="225"/>
+      <c r="O3" s="226"/>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="216"/>
-      <c r="C4" s="217"/>
-      <c r="D4" s="217"/>
-      <c r="E4" s="217"/>
-      <c r="F4" s="217"/>
-      <c r="G4" s="218"/>
-      <c r="H4" s="222" t="s">
+      <c r="B4" s="218"/>
+      <c r="C4" s="219"/>
+      <c r="D4" s="219"/>
+      <c r="E4" s="219"/>
+      <c r="F4" s="219"/>
+      <c r="G4" s="220"/>
+      <c r="H4" s="224" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="223"/>
-      <c r="J4" s="223"/>
-      <c r="K4" s="223"/>
-      <c r="L4" s="223"/>
-      <c r="M4" s="223"/>
-      <c r="N4" s="223"/>
-      <c r="O4" s="224"/>
+      <c r="I4" s="225"/>
+      <c r="J4" s="225"/>
+      <c r="K4" s="225"/>
+      <c r="L4" s="225"/>
+      <c r="M4" s="225"/>
+      <c r="N4" s="225"/>
+      <c r="O4" s="226"/>
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="216"/>
-      <c r="C5" s="217"/>
-      <c r="D5" s="217"/>
-      <c r="E5" s="217"/>
-      <c r="F5" s="217"/>
-      <c r="G5" s="218"/>
-      <c r="H5" s="225" t="s">
+      <c r="B5" s="218"/>
+      <c r="C5" s="219"/>
+      <c r="D5" s="219"/>
+      <c r="E5" s="219"/>
+      <c r="F5" s="219"/>
+      <c r="G5" s="220"/>
+      <c r="H5" s="227" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="226"/>
-      <c r="J5" s="226"/>
-      <c r="K5" s="226"/>
-      <c r="L5" s="226"/>
-      <c r="M5" s="226"/>
-      <c r="N5" s="226"/>
-      <c r="O5" s="227"/>
+      <c r="I5" s="228"/>
+      <c r="J5" s="228"/>
+      <c r="K5" s="228"/>
+      <c r="L5" s="228"/>
+      <c r="M5" s="228"/>
+      <c r="N5" s="228"/>
+      <c r="O5" s="229"/>
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
-      <c r="B6" s="232" t="s">
+      <c r="B6" s="234" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="233"/>
-      <c r="D6" s="233"/>
-      <c r="E6" s="233"/>
-      <c r="F6" s="233"/>
-      <c r="G6" s="234"/>
+      <c r="C6" s="235"/>
+      <c r="D6" s="235"/>
+      <c r="E6" s="235"/>
+      <c r="F6" s="235"/>
+      <c r="G6" s="236"/>
       <c r="H6" s="6"/>
       <c r="I6" s="7"/>
       <c r="J6" s="8"/>
@@ -4691,12 +4691,12 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="235"/>
-      <c r="C7" s="233"/>
-      <c r="D7" s="233"/>
-      <c r="E7" s="233"/>
-      <c r="F7" s="233"/>
-      <c r="G7" s="234"/>
+      <c r="B7" s="237"/>
+      <c r="C7" s="235"/>
+      <c r="D7" s="235"/>
+      <c r="E7" s="235"/>
+      <c r="F7" s="235"/>
+      <c r="G7" s="236"/>
       <c r="H7" s="10" t="s">
         <v>5</v>
       </c>
@@ -4715,12 +4715,12 @@
     </row>
     <row r="8" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="236"/>
-      <c r="C8" s="237"/>
-      <c r="D8" s="237"/>
-      <c r="E8" s="237"/>
-      <c r="F8" s="237"/>
-      <c r="G8" s="238"/>
+      <c r="B8" s="238"/>
+      <c r="C8" s="239"/>
+      <c r="D8" s="239"/>
+      <c r="E8" s="239"/>
+      <c r="F8" s="239"/>
+      <c r="G8" s="240"/>
       <c r="H8" s="16" t="s">
         <v>8</v>
       </c>
@@ -4759,22 +4759,22 @@
     </row>
     <row r="10" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
-      <c r="B10" s="239" t="s">
+      <c r="B10" s="241" t="s">
         <v>267</v>
       </c>
-      <c r="C10" s="240"/>
-      <c r="D10" s="240"/>
-      <c r="E10" s="240"/>
-      <c r="F10" s="240"/>
-      <c r="G10" s="240"/>
-      <c r="H10" s="240"/>
-      <c r="I10" s="240"/>
-      <c r="J10" s="240"/>
-      <c r="K10" s="240"/>
-      <c r="L10" s="240"/>
-      <c r="M10" s="240"/>
-      <c r="N10" s="240"/>
-      <c r="O10" s="241"/>
+      <c r="C10" s="242"/>
+      <c r="D10" s="242"/>
+      <c r="E10" s="242"/>
+      <c r="F10" s="242"/>
+      <c r="G10" s="242"/>
+      <c r="H10" s="242"/>
+      <c r="I10" s="242"/>
+      <c r="J10" s="242"/>
+      <c r="K10" s="242"/>
+      <c r="L10" s="242"/>
+      <c r="M10" s="242"/>
+      <c r="N10" s="242"/>
+      <c r="O10" s="243"/>
       <c r="P10" s="21"/>
     </row>
     <row r="11" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4826,12 +4826,12 @@
       <c r="J13" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="242" t="s">
+      <c r="K13" s="244" t="s">
         <v>289</v>
       </c>
-      <c r="L13" s="242"/>
-      <c r="M13" s="242"/>
-      <c r="N13" s="243"/>
+      <c r="L13" s="244"/>
+      <c r="M13" s="244"/>
+      <c r="N13" s="245"/>
       <c r="O13" s="31"/>
       <c r="P13" s="21"/>
     </row>
@@ -5520,8 +5520,8 @@
       <c r="K49" s="55"/>
       <c r="L49" s="52"/>
       <c r="M49" s="52"/>
-      <c r="N49" s="244"/>
-      <c r="O49" s="245"/>
+      <c r="N49" s="246"/>
+      <c r="O49" s="247"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B50" s="56"/>
@@ -5536,8 +5536,8 @@
       <c r="K50" s="61"/>
       <c r="L50" s="59"/>
       <c r="M50" s="59"/>
-      <c r="N50" s="211"/>
-      <c r="O50" s="212"/>
+      <c r="N50" s="213"/>
+      <c r="O50" s="214"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B51" s="62"/>
@@ -5552,8 +5552,8 @@
       <c r="K51" s="61"/>
       <c r="L51" s="59"/>
       <c r="M51" s="59"/>
-      <c r="N51" s="211"/>
-      <c r="O51" s="212"/>
+      <c r="N51" s="213"/>
+      <c r="O51" s="214"/>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B52" s="62"/>
@@ -5568,8 +5568,8 @@
       <c r="K52" s="61"/>
       <c r="L52" s="59"/>
       <c r="M52" s="59"/>
-      <c r="N52" s="211"/>
-      <c r="O52" s="212"/>
+      <c r="N52" s="213"/>
+      <c r="O52" s="214"/>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B53" s="62"/>
@@ -5584,8 +5584,8 @@
       <c r="K53" s="61"/>
       <c r="L53" s="59"/>
       <c r="M53" s="59"/>
-      <c r="N53" s="211"/>
-      <c r="O53" s="212"/>
+      <c r="N53" s="213"/>
+      <c r="O53" s="214"/>
     </row>
     <row r="54" spans="2:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B54" s="66"/>
@@ -5600,17 +5600,17 @@
       <c r="K54" s="72"/>
       <c r="L54" s="69"/>
       <c r="M54" s="69"/>
-      <c r="N54" s="228"/>
-      <c r="O54" s="229"/>
+      <c r="N54" s="230"/>
+      <c r="O54" s="231"/>
     </row>
     <row r="55" spans="2:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B55" s="66" t="s">
         <v>295</v>
       </c>
-      <c r="C55" s="325">
+      <c r="C55" s="211">
         <v>42136</v>
       </c>
-      <c r="D55" s="326"/>
+      <c r="D55" s="212"/>
       <c r="E55" s="69">
         <v>4</v>
       </c>
@@ -5628,10 +5628,10 @@
       <c r="M55" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="N55" s="230" t="s">
+      <c r="N55" s="232" t="s">
         <v>293</v>
       </c>
-      <c r="O55" s="231"/>
+      <c r="O55" s="233"/>
     </row>
     <row r="56" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B56" s="74" t="s">
@@ -5695,8 +5695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R568"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138:D138"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5727,10 +5727,10 @@
       <c r="C1" s="86"/>
       <c r="D1" s="86"/>
       <c r="E1" s="86"/>
-      <c r="F1" s="248" t="s">
+      <c r="F1" s="250" t="s">
         <v>252</v>
       </c>
-      <c r="G1" s="249"/>
+      <c r="G1" s="251"/>
       <c r="H1" s="86"/>
       <c r="I1" s="86"/>
       <c r="J1" s="86"/>
@@ -5745,8 +5745,8 @@
       <c r="C2" s="92"/>
       <c r="D2" s="92"/>
       <c r="E2" s="92"/>
-      <c r="F2" s="250"/>
-      <c r="G2" s="251"/>
+      <c r="F2" s="252"/>
+      <c r="G2" s="253"/>
       <c r="H2" s="123"/>
       <c r="I2" s="123"/>
       <c r="J2" s="123"/>
@@ -5763,8 +5763,8 @@
       <c r="C3" s="201"/>
       <c r="D3" s="201"/>
       <c r="E3" s="201"/>
-      <c r="F3" s="250"/>
-      <c r="G3" s="251"/>
+      <c r="F3" s="252"/>
+      <c r="G3" s="253"/>
       <c r="H3" s="124"/>
       <c r="I3" s="124"/>
       <c r="J3" s="124"/>
@@ -5780,8 +5780,8 @@
       <c r="C4" s="201"/>
       <c r="D4" s="201"/>
       <c r="E4" s="201"/>
-      <c r="F4" s="250"/>
-      <c r="G4" s="251"/>
+      <c r="F4" s="252"/>
+      <c r="G4" s="253"/>
       <c r="H4" s="125"/>
       <c r="I4" s="125"/>
       <c r="J4" s="125"/>
@@ -5797,8 +5797,8 @@
       <c r="C5" s="84"/>
       <c r="D5" s="84"/>
       <c r="E5" s="84"/>
-      <c r="F5" s="252"/>
-      <c r="G5" s="253"/>
+      <c r="F5" s="254"/>
+      <c r="G5" s="255"/>
       <c r="H5" s="126"/>
       <c r="I5" s="126"/>
       <c r="J5" s="126"/>
@@ -5811,105 +5811,105 @@
       <c r="R5" s="89"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="246" t="s">
+      <c r="A6" s="248" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="247"/>
+      <c r="B6" s="249"/>
       <c r="C6" s="99"/>
-      <c r="D6" s="260" t="s">
+      <c r="D6" s="262" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="261"/>
-      <c r="F6" s="261"/>
-      <c r="G6" s="262"/>
+      <c r="E6" s="263"/>
+      <c r="F6" s="263"/>
+      <c r="G6" s="264"/>
       <c r="H6" s="174" t="s">
         <v>258</v>
       </c>
-      <c r="I6" s="310" t="s">
+      <c r="I6" s="315" t="s">
         <v>289</v>
       </c>
-      <c r="J6" s="311"/>
-      <c r="K6" s="311"/>
-      <c r="L6" s="312"/>
-      <c r="M6" s="313" t="s">
+      <c r="J6" s="316"/>
+      <c r="K6" s="316"/>
+      <c r="L6" s="317"/>
+      <c r="M6" s="318" t="s">
         <v>294</v>
       </c>
-      <c r="N6" s="314"/>
+      <c r="N6" s="319"/>
       <c r="O6" s="116"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="280" t="s">
+      <c r="A7" s="282" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="281"/>
+      <c r="B7" s="283"/>
       <c r="C7" s="99"/>
-      <c r="D7" s="257" t="s">
+      <c r="D7" s="259" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="258"/>
-      <c r="F7" s="258"/>
-      <c r="G7" s="259"/>
+      <c r="E7" s="260"/>
+      <c r="F7" s="260"/>
+      <c r="G7" s="261"/>
       <c r="H7" s="142" t="s">
         <v>259</v>
       </c>
-      <c r="I7" s="315"/>
-      <c r="J7" s="315"/>
-      <c r="K7" s="315"/>
-      <c r="L7" s="315"/>
-      <c r="M7" s="313"/>
-      <c r="N7" s="314"/>
+      <c r="I7" s="320"/>
+      <c r="J7" s="320"/>
+      <c r="K7" s="320"/>
+      <c r="L7" s="320"/>
+      <c r="M7" s="318"/>
+      <c r="N7" s="319"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="280" t="s">
+      <c r="A8" s="282" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="281"/>
+      <c r="B8" s="283"/>
       <c r="C8" s="99"/>
-      <c r="D8" s="257" t="s">
+      <c r="D8" s="259" t="s">
         <v>269</v>
       </c>
-      <c r="E8" s="258"/>
-      <c r="F8" s="258"/>
-      <c r="G8" s="259"/>
+      <c r="E8" s="260"/>
+      <c r="F8" s="260"/>
+      <c r="G8" s="261"/>
       <c r="H8" s="143" t="s">
         <v>255</v>
       </c>
-      <c r="I8" s="316" t="s">
+      <c r="I8" s="321" t="s">
         <v>256</v>
       </c>
-      <c r="J8" s="316"/>
-      <c r="K8" s="316"/>
-      <c r="L8" s="316"/>
-      <c r="M8" s="313"/>
-      <c r="N8" s="314"/>
+      <c r="J8" s="321"/>
+      <c r="K8" s="321"/>
+      <c r="L8" s="321"/>
+      <c r="M8" s="318"/>
+      <c r="N8" s="319"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="280" t="s">
+      <c r="A9" s="282" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="281"/>
+      <c r="B9" s="283"/>
       <c r="C9" s="99"/>
-      <c r="D9" s="254">
-        <v>240</v>
-      </c>
-      <c r="E9" s="255"/>
-      <c r="F9" s="255"/>
-      <c r="G9" s="256"/>
+      <c r="D9" s="256">
+        <v>240</v>
+      </c>
+      <c r="E9" s="257"/>
+      <c r="F9" s="257"/>
+      <c r="G9" s="258"/>
       <c r="H9" s="143" t="s">
         <v>257</v>
       </c>
-      <c r="I9" s="316" t="s">
+      <c r="I9" s="321" t="s">
         <v>256</v>
       </c>
-      <c r="J9" s="316"/>
-      <c r="K9" s="316"/>
-      <c r="L9" s="316"/>
+      <c r="J9" s="321"/>
+      <c r="K9" s="321"/>
+      <c r="L9" s="321"/>
       <c r="M9" s="98"/>
       <c r="N9" s="132"/>
     </row>
     <row r="10" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="272"/>
-      <c r="B10" s="273"/>
+      <c r="A10" s="274"/>
+      <c r="B10" s="275"/>
       <c r="C10" s="100"/>
       <c r="D10" s="201"/>
       <c r="E10" s="201"/>
@@ -5930,11 +5930,11 @@
       <c r="B11" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="274" t="s">
+      <c r="C11" s="276" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="275"/>
-      <c r="E11" s="276"/>
+      <c r="D11" s="277"/>
+      <c r="E11" s="278"/>
       <c r="F11" s="107" t="s">
         <v>234</v>
       </c>
@@ -5967,9 +5967,9 @@
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="134"/>
       <c r="B12" s="104"/>
-      <c r="C12" s="277"/>
-      <c r="D12" s="278"/>
-      <c r="E12" s="279"/>
+      <c r="C12" s="279"/>
+      <c r="D12" s="280"/>
+      <c r="E12" s="281"/>
       <c r="F12" s="201"/>
       <c r="G12" s="201"/>
       <c r="H12" s="103"/>
@@ -5988,11 +5988,11 @@
       <c r="B13" s="167" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="266" t="s">
+      <c r="C13" s="268" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="267"/>
-      <c r="E13" s="268"/>
+      <c r="D13" s="269"/>
+      <c r="E13" s="270"/>
       <c r="F13" s="167" t="s">
         <v>70</v>
       </c>
@@ -6029,11 +6029,11 @@
       <c r="B14" s="167" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="266" t="s">
+      <c r="C14" s="268" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="267"/>
-      <c r="E14" s="268"/>
+      <c r="D14" s="269"/>
+      <c r="E14" s="270"/>
       <c r="F14" s="167" t="s">
         <v>72</v>
       </c>
@@ -6070,11 +6070,11 @@
       <c r="B15" s="152" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="266" t="s">
+      <c r="C15" s="268" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="267"/>
-      <c r="E15" s="268"/>
+      <c r="D15" s="269"/>
+      <c r="E15" s="270"/>
       <c r="F15" s="167" t="s">
         <v>96</v>
       </c>
@@ -6111,11 +6111,11 @@
       <c r="B16" s="152" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="266" t="s">
+      <c r="C16" s="268" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="267"/>
-      <c r="E16" s="268"/>
+      <c r="D16" s="269"/>
+      <c r="E16" s="270"/>
       <c r="F16" s="167" t="s">
         <v>89</v>
       </c>
@@ -6146,11 +6146,11 @@
         <v>5</v>
       </c>
       <c r="B17" s="153"/>
-      <c r="C17" s="266" t="s">
+      <c r="C17" s="268" t="s">
         <v>98</v>
       </c>
-      <c r="D17" s="267"/>
-      <c r="E17" s="268"/>
+      <c r="D17" s="269"/>
+      <c r="E17" s="270"/>
       <c r="F17" s="154"/>
       <c r="G17" s="153"/>
       <c r="H17" s="163" t="s">
@@ -6181,11 +6181,11 @@
         <v>6</v>
       </c>
       <c r="B18" s="153"/>
-      <c r="C18" s="266" t="s">
+      <c r="C18" s="268" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="267"/>
-      <c r="E18" s="268"/>
+      <c r="D18" s="269"/>
+      <c r="E18" s="270"/>
       <c r="F18" s="154"/>
       <c r="G18" s="153"/>
       <c r="H18" s="163" t="s">
@@ -6216,11 +6216,11 @@
         <v>7</v>
       </c>
       <c r="B19" s="153"/>
-      <c r="C19" s="266" t="s">
+      <c r="C19" s="268" t="s">
         <v>104</v>
       </c>
-      <c r="D19" s="267"/>
-      <c r="E19" s="268"/>
+      <c r="D19" s="269"/>
+      <c r="E19" s="270"/>
       <c r="F19" s="154"/>
       <c r="G19" s="153"/>
       <c r="H19" s="163" t="s">
@@ -6251,11 +6251,11 @@
         <v>8</v>
       </c>
       <c r="B20" s="153"/>
-      <c r="C20" s="266" t="s">
+      <c r="C20" s="268" t="s">
         <v>105</v>
       </c>
-      <c r="D20" s="267"/>
-      <c r="E20" s="268"/>
+      <c r="D20" s="269"/>
+      <c r="E20" s="270"/>
       <c r="F20" s="154"/>
       <c r="G20" s="153"/>
       <c r="H20" s="163" t="s">
@@ -6286,11 +6286,11 @@
         <v>9</v>
       </c>
       <c r="B21" s="153"/>
-      <c r="C21" s="266" t="s">
+      <c r="C21" s="268" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="267"/>
-      <c r="E21" s="268"/>
+      <c r="D21" s="269"/>
+      <c r="E21" s="270"/>
       <c r="F21" s="154"/>
       <c r="G21" s="153"/>
       <c r="H21" s="163" t="s">
@@ -6323,11 +6323,11 @@
       <c r="B22" s="193" t="s">
         <v>107</v>
       </c>
-      <c r="C22" s="266" t="s">
+      <c r="C22" s="268" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="267"/>
-      <c r="E22" s="268"/>
+      <c r="D22" s="269"/>
+      <c r="E22" s="270"/>
       <c r="F22" s="163" t="s">
         <v>71</v>
       </c>
@@ -6364,11 +6364,11 @@
       <c r="B23" s="193" t="s">
         <v>109</v>
       </c>
-      <c r="C23" s="266" t="s">
+      <c r="C23" s="268" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="267"/>
-      <c r="E23" s="268"/>
+      <c r="D23" s="269"/>
+      <c r="E23" s="270"/>
       <c r="F23" s="163" t="s">
         <v>71</v>
       </c>
@@ -6405,11 +6405,11 @@
       <c r="B24" s="193" t="s">
         <v>110</v>
       </c>
-      <c r="C24" s="266" t="s">
+      <c r="C24" s="268" t="s">
         <v>108</v>
       </c>
-      <c r="D24" s="267"/>
-      <c r="E24" s="268"/>
+      <c r="D24" s="269"/>
+      <c r="E24" s="270"/>
       <c r="F24" s="163" t="s">
         <v>71</v>
       </c>
@@ -6444,11 +6444,11 @@
         <v>13</v>
       </c>
       <c r="B25" s="152"/>
-      <c r="C25" s="266" t="s">
+      <c r="C25" s="268" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="267"/>
-      <c r="E25" s="268"/>
+      <c r="D25" s="269"/>
+      <c r="E25" s="270"/>
       <c r="F25" s="163" t="s">
         <v>71</v>
       </c>
@@ -6483,11 +6483,11 @@
         <v>14</v>
       </c>
       <c r="B26" s="153"/>
-      <c r="C26" s="266" t="s">
+      <c r="C26" s="268" t="s">
         <v>114</v>
       </c>
-      <c r="D26" s="267"/>
-      <c r="E26" s="268"/>
+      <c r="D26" s="269"/>
+      <c r="E26" s="270"/>
       <c r="F26" s="163" t="s">
         <v>71</v>
       </c>
@@ -6518,17 +6518,17 @@
       <c r="O26" s="78"/>
     </row>
     <row r="27" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="263">
+      <c r="A27" s="265">
         <v>15</v>
       </c>
       <c r="B27" s="155" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="269" t="s">
+      <c r="C27" s="271" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="270"/>
-      <c r="E27" s="271"/>
+      <c r="D27" s="272"/>
+      <c r="E27" s="273"/>
       <c r="F27" s="167" t="s">
         <v>71</v>
       </c>
@@ -6559,15 +6559,15 @@
       <c r="O27" s="78"/>
     </row>
     <row r="28" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="265"/>
+      <c r="A28" s="267"/>
       <c r="B28" s="156" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="269" t="s">
+      <c r="C28" s="271" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="270"/>
-      <c r="E28" s="271"/>
+      <c r="D28" s="272"/>
+      <c r="E28" s="273"/>
       <c r="F28" s="167" t="s">
         <v>71</v>
       </c>
@@ -6598,17 +6598,17 @@
       <c r="O28" s="78"/>
     </row>
     <row r="29" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="263">
+      <c r="A29" s="265">
         <v>16</v>
       </c>
       <c r="B29" s="152" t="s">
         <v>118</v>
       </c>
-      <c r="C29" s="269" t="s">
+      <c r="C29" s="271" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="270"/>
-      <c r="E29" s="271"/>
+      <c r="D29" s="272"/>
+      <c r="E29" s="273"/>
       <c r="F29" s="167" t="s">
         <v>71</v>
       </c>
@@ -6637,15 +6637,15 @@
       <c r="O29" s="78"/>
     </row>
     <row r="30" spans="1:17" s="194" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="265"/>
+      <c r="A30" s="267"/>
       <c r="B30" s="198" t="s">
         <v>120</v>
       </c>
-      <c r="C30" s="269" t="s">
+      <c r="C30" s="271" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="270"/>
-      <c r="E30" s="271"/>
+      <c r="D30" s="272"/>
+      <c r="E30" s="273"/>
       <c r="F30" s="167" t="s">
         <v>71</v>
       </c>
@@ -6676,17 +6676,17 @@
       <c r="Q30" s="117"/>
     </row>
     <row r="31" spans="1:17" s="79" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="263">
+      <c r="A31" s="265">
         <v>17</v>
       </c>
       <c r="B31" s="156" t="s">
         <v>121</v>
       </c>
-      <c r="C31" s="269" t="s">
+      <c r="C31" s="271" t="s">
         <v>122</v>
       </c>
-      <c r="D31" s="270"/>
-      <c r="E31" s="271"/>
+      <c r="D31" s="272"/>
+      <c r="E31" s="273"/>
       <c r="F31" s="167" t="s">
         <v>71</v>
       </c>
@@ -6719,15 +6719,15 @@
       <c r="Q31" s="117"/>
     </row>
     <row r="32" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="265"/>
+      <c r="A32" s="267"/>
       <c r="B32" s="156" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="269" t="s">
+      <c r="C32" s="271" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="270"/>
-      <c r="E32" s="271"/>
+      <c r="D32" s="272"/>
+      <c r="E32" s="273"/>
       <c r="F32" s="167" t="s">
         <v>71</v>
       </c>
@@ -6758,17 +6758,17 @@
       <c r="O32" s="78"/>
     </row>
     <row r="33" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="263">
+      <c r="A33" s="265">
         <v>18</v>
       </c>
       <c r="B33" s="198" t="s">
         <v>206</v>
       </c>
-      <c r="C33" s="269" t="s">
+      <c r="C33" s="271" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="270"/>
-      <c r="E33" s="271"/>
+      <c r="D33" s="272"/>
+      <c r="E33" s="273"/>
       <c r="F33" s="167" t="s">
         <v>71</v>
       </c>
@@ -6797,15 +6797,15 @@
       <c r="O33" s="78"/>
     </row>
     <row r="34" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="265"/>
+      <c r="A34" s="267"/>
       <c r="B34" s="198" t="s">
         <v>207</v>
       </c>
-      <c r="C34" s="269" t="s">
+      <c r="C34" s="271" t="s">
         <v>124</v>
       </c>
-      <c r="D34" s="270"/>
-      <c r="E34" s="271"/>
+      <c r="D34" s="272"/>
+      <c r="E34" s="273"/>
       <c r="F34" s="167" t="s">
         <v>71</v>
       </c>
@@ -6834,17 +6834,17 @@
       <c r="O34" s="78"/>
     </row>
     <row r="35" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="263">
+      <c r="A35" s="265">
         <v>19</v>
       </c>
       <c r="B35" s="156" t="s">
         <v>125</v>
       </c>
-      <c r="C35" s="269" t="s">
+      <c r="C35" s="271" t="s">
         <v>126</v>
       </c>
-      <c r="D35" s="270"/>
-      <c r="E35" s="271"/>
+      <c r="D35" s="272"/>
+      <c r="E35" s="273"/>
       <c r="F35" s="167" t="s">
         <v>71</v>
       </c>
@@ -6875,15 +6875,15 @@
       <c r="O35" s="78"/>
     </row>
     <row r="36" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="265"/>
+      <c r="A36" s="267"/>
       <c r="B36" s="198" t="s">
         <v>128</v>
       </c>
-      <c r="C36" s="269" t="s">
+      <c r="C36" s="271" t="s">
         <v>129</v>
       </c>
-      <c r="D36" s="270"/>
-      <c r="E36" s="271"/>
+      <c r="D36" s="272"/>
+      <c r="E36" s="273"/>
       <c r="F36" s="167" t="s">
         <v>71</v>
       </c>
@@ -6912,17 +6912,17 @@
       <c r="O36" s="78"/>
     </row>
     <row r="37" spans="1:15" s="117" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="303">
+      <c r="A37" s="308">
         <v>20</v>
       </c>
       <c r="B37" s="156" t="s">
         <v>130</v>
       </c>
-      <c r="C37" s="269" t="s">
+      <c r="C37" s="271" t="s">
         <v>126</v>
       </c>
-      <c r="D37" s="270"/>
-      <c r="E37" s="271"/>
+      <c r="D37" s="272"/>
+      <c r="E37" s="273"/>
       <c r="F37" s="167" t="s">
         <v>71</v>
       </c>
@@ -6952,15 +6952,15 @@
       </c>
     </row>
     <row r="38" spans="1:15" s="117" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="304"/>
+      <c r="A38" s="309"/>
       <c r="B38" s="198" t="s">
         <v>131</v>
       </c>
-      <c r="C38" s="269" t="s">
+      <c r="C38" s="271" t="s">
         <v>129</v>
       </c>
-      <c r="D38" s="270"/>
-      <c r="E38" s="271"/>
+      <c r="D38" s="272"/>
+      <c r="E38" s="273"/>
       <c r="F38" s="167" t="s">
         <v>71</v>
       </c>
@@ -6988,17 +6988,17 @@
       <c r="N38" s="136"/>
     </row>
     <row r="39" spans="1:15" s="117" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="303">
+      <c r="A39" s="308">
         <v>21</v>
       </c>
       <c r="B39" s="156" t="s">
         <v>132</v>
       </c>
-      <c r="C39" s="269" t="s">
+      <c r="C39" s="271" t="s">
         <v>126</v>
       </c>
-      <c r="D39" s="270"/>
-      <c r="E39" s="271"/>
+      <c r="D39" s="272"/>
+      <c r="E39" s="273"/>
       <c r="F39" s="167" t="s">
         <v>71</v>
       </c>
@@ -7028,15 +7028,15 @@
       </c>
     </row>
     <row r="40" spans="1:15" s="117" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="304"/>
+      <c r="A40" s="309"/>
       <c r="B40" s="198" t="s">
         <v>133</v>
       </c>
-      <c r="C40" s="269" t="s">
+      <c r="C40" s="271" t="s">
         <v>129</v>
       </c>
-      <c r="D40" s="270"/>
-      <c r="E40" s="271"/>
+      <c r="D40" s="272"/>
+      <c r="E40" s="273"/>
       <c r="F40" s="167" t="s">
         <v>71</v>
       </c>
@@ -7064,17 +7064,17 @@
       <c r="N40" s="136"/>
     </row>
     <row r="41" spans="1:15" s="117" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="263">
+      <c r="A41" s="265">
         <v>22</v>
       </c>
       <c r="B41" s="156" t="s">
         <v>134</v>
       </c>
-      <c r="C41" s="269" t="s">
+      <c r="C41" s="271" t="s">
         <v>126</v>
       </c>
-      <c r="D41" s="270"/>
-      <c r="E41" s="271"/>
+      <c r="D41" s="272"/>
+      <c r="E41" s="273"/>
       <c r="F41" s="167" t="s">
         <v>71</v>
       </c>
@@ -7104,15 +7104,15 @@
       </c>
     </row>
     <row r="42" spans="1:15" s="79" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="265"/>
+      <c r="A42" s="267"/>
       <c r="B42" s="198" t="s">
         <v>135</v>
       </c>
-      <c r="C42" s="269" t="s">
+      <c r="C42" s="271" t="s">
         <v>129</v>
       </c>
-      <c r="D42" s="270"/>
-      <c r="E42" s="271"/>
+      <c r="D42" s="272"/>
+      <c r="E42" s="273"/>
       <c r="F42" s="167" t="s">
         <v>71</v>
       </c>
@@ -7140,17 +7140,17 @@
       <c r="N42" s="136"/>
     </row>
     <row r="43" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="263">
+      <c r="A43" s="265">
         <v>23</v>
       </c>
       <c r="B43" s="198" t="s">
         <v>136</v>
       </c>
-      <c r="C43" s="269" t="s">
+      <c r="C43" s="271" t="s">
         <v>137</v>
       </c>
-      <c r="D43" s="270"/>
-      <c r="E43" s="271"/>
+      <c r="D43" s="272"/>
+      <c r="E43" s="273"/>
       <c r="F43" s="167" t="s">
         <v>71</v>
       </c>
@@ -7181,15 +7181,15 @@
       <c r="O43" s="78"/>
     </row>
     <row r="44" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="265"/>
+      <c r="A44" s="267"/>
       <c r="B44" s="198" t="s">
         <v>138</v>
       </c>
-      <c r="C44" s="269" t="s">
+      <c r="C44" s="271" t="s">
         <v>139</v>
       </c>
-      <c r="D44" s="270"/>
-      <c r="E44" s="271"/>
+      <c r="D44" s="272"/>
+      <c r="E44" s="273"/>
       <c r="F44" s="167" t="s">
         <v>71</v>
       </c>
@@ -7218,17 +7218,17 @@
       <c r="O44" s="78"/>
     </row>
     <row r="45" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="263">
+      <c r="A45" s="265">
         <v>24</v>
       </c>
       <c r="B45" s="198" t="s">
         <v>140</v>
       </c>
-      <c r="C45" s="269" t="s">
+      <c r="C45" s="271" t="s">
         <v>137</v>
       </c>
-      <c r="D45" s="270"/>
-      <c r="E45" s="271"/>
+      <c r="D45" s="272"/>
+      <c r="E45" s="273"/>
       <c r="F45" s="167" t="s">
         <v>71</v>
       </c>
@@ -7259,15 +7259,15 @@
       <c r="O45" s="78"/>
     </row>
     <row r="46" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="265"/>
+      <c r="A46" s="267"/>
       <c r="B46" s="198" t="s">
         <v>141</v>
       </c>
-      <c r="C46" s="269" t="s">
+      <c r="C46" s="271" t="s">
         <v>139</v>
       </c>
-      <c r="D46" s="270"/>
-      <c r="E46" s="271"/>
+      <c r="D46" s="272"/>
+      <c r="E46" s="273"/>
       <c r="F46" s="167" t="s">
         <v>71</v>
       </c>
@@ -7296,17 +7296,17 @@
       <c r="O46" s="78"/>
     </row>
     <row r="47" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="263">
+      <c r="A47" s="265">
         <v>25</v>
       </c>
       <c r="B47" s="198" t="s">
         <v>142</v>
       </c>
-      <c r="C47" s="269" t="s">
+      <c r="C47" s="271" t="s">
         <v>137</v>
       </c>
-      <c r="D47" s="270"/>
-      <c r="E47" s="271"/>
+      <c r="D47" s="272"/>
+      <c r="E47" s="273"/>
       <c r="F47" s="167" t="s">
         <v>71</v>
       </c>
@@ -7337,15 +7337,15 @@
       <c r="O47" s="78"/>
     </row>
     <row r="48" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="265"/>
+      <c r="A48" s="267"/>
       <c r="B48" s="198" t="s">
         <v>143</v>
       </c>
-      <c r="C48" s="269" t="s">
+      <c r="C48" s="271" t="s">
         <v>139</v>
       </c>
-      <c r="D48" s="270"/>
-      <c r="E48" s="271"/>
+      <c r="D48" s="272"/>
+      <c r="E48" s="273"/>
       <c r="F48" s="167" t="s">
         <v>71</v>
       </c>
@@ -7374,17 +7374,17 @@
       <c r="O48" s="78"/>
     </row>
     <row r="49" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="263">
+      <c r="A49" s="265">
         <v>26</v>
       </c>
       <c r="B49" s="198" t="s">
         <v>144</v>
       </c>
-      <c r="C49" s="269" t="s">
+      <c r="C49" s="271" t="s">
         <v>137</v>
       </c>
-      <c r="D49" s="270"/>
-      <c r="E49" s="271"/>
+      <c r="D49" s="272"/>
+      <c r="E49" s="273"/>
       <c r="F49" s="167" t="s">
         <v>71</v>
       </c>
@@ -7415,15 +7415,15 @@
       <c r="O49" s="78"/>
     </row>
     <row r="50" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="265"/>
+      <c r="A50" s="267"/>
       <c r="B50" s="198" t="s">
         <v>145</v>
       </c>
-      <c r="C50" s="269" t="s">
+      <c r="C50" s="271" t="s">
         <v>139</v>
       </c>
-      <c r="D50" s="270"/>
-      <c r="E50" s="271"/>
+      <c r="D50" s="272"/>
+      <c r="E50" s="273"/>
       <c r="F50" s="167" t="s">
         <v>71</v>
       </c>
@@ -7452,17 +7452,17 @@
       <c r="O50" s="78"/>
     </row>
     <row r="51" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="263">
+      <c r="A51" s="265">
         <v>27</v>
       </c>
       <c r="B51" s="198" t="s">
         <v>146</v>
       </c>
-      <c r="C51" s="269" t="s">
+      <c r="C51" s="271" t="s">
         <v>147</v>
       </c>
-      <c r="D51" s="270"/>
-      <c r="E51" s="271"/>
+      <c r="D51" s="272"/>
+      <c r="E51" s="273"/>
       <c r="F51" s="167" t="s">
         <v>71</v>
       </c>
@@ -7493,15 +7493,15 @@
       <c r="O51" s="78"/>
     </row>
     <row r="52" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="265"/>
+      <c r="A52" s="267"/>
       <c r="B52" s="198" t="s">
         <v>148</v>
       </c>
-      <c r="C52" s="269" t="s">
+      <c r="C52" s="271" t="s">
         <v>149</v>
       </c>
-      <c r="D52" s="270"/>
-      <c r="E52" s="271"/>
+      <c r="D52" s="272"/>
+      <c r="E52" s="273"/>
       <c r="F52" s="167" t="s">
         <v>71</v>
       </c>
@@ -7530,17 +7530,17 @@
       <c r="O52" s="78"/>
     </row>
     <row r="53" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="305">
+      <c r="A53" s="310">
         <v>28</v>
       </c>
       <c r="B53" s="198" t="s">
         <v>150</v>
       </c>
-      <c r="C53" s="269" t="s">
+      <c r="C53" s="271" t="s">
         <v>147</v>
       </c>
-      <c r="D53" s="270"/>
-      <c r="E53" s="271"/>
+      <c r="D53" s="272"/>
+      <c r="E53" s="273"/>
       <c r="F53" s="167" t="s">
         <v>71</v>
       </c>
@@ -7571,15 +7571,15 @@
       <c r="O53" s="78"/>
     </row>
     <row r="54" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="306"/>
+      <c r="A54" s="311"/>
       <c r="B54" s="198" t="s">
         <v>151</v>
       </c>
-      <c r="C54" s="269" t="s">
+      <c r="C54" s="271" t="s">
         <v>149</v>
       </c>
-      <c r="D54" s="270"/>
-      <c r="E54" s="271"/>
+      <c r="D54" s="272"/>
+      <c r="E54" s="273"/>
       <c r="F54" s="167" t="s">
         <v>71</v>
       </c>
@@ -7608,17 +7608,17 @@
       <c r="O54" s="78"/>
     </row>
     <row r="55" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="263">
+      <c r="A55" s="265">
         <v>29</v>
       </c>
       <c r="B55" s="198" t="s">
         <v>152</v>
       </c>
-      <c r="C55" s="269" t="s">
+      <c r="C55" s="271" t="s">
         <v>147</v>
       </c>
-      <c r="D55" s="270"/>
-      <c r="E55" s="271"/>
+      <c r="D55" s="272"/>
+      <c r="E55" s="273"/>
       <c r="F55" s="167" t="s">
         <v>71</v>
       </c>
@@ -7649,15 +7649,15 @@
       <c r="O55" s="78"/>
     </row>
     <row r="56" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="265"/>
+      <c r="A56" s="267"/>
       <c r="B56" s="198" t="s">
         <v>153</v>
       </c>
-      <c r="C56" s="269" t="s">
+      <c r="C56" s="271" t="s">
         <v>149</v>
       </c>
-      <c r="D56" s="270"/>
-      <c r="E56" s="271"/>
+      <c r="D56" s="272"/>
+      <c r="E56" s="273"/>
       <c r="F56" s="167" t="s">
         <v>71</v>
       </c>
@@ -7686,17 +7686,17 @@
       <c r="O56" s="78"/>
     </row>
     <row r="57" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="263">
+      <c r="A57" s="265">
         <v>30</v>
       </c>
       <c r="B57" s="198" t="s">
         <v>154</v>
       </c>
-      <c r="C57" s="269" t="s">
+      <c r="C57" s="271" t="s">
         <v>147</v>
       </c>
-      <c r="D57" s="270"/>
-      <c r="E57" s="271"/>
+      <c r="D57" s="272"/>
+      <c r="E57" s="273"/>
       <c r="F57" s="167" t="s">
         <v>71</v>
       </c>
@@ -7727,15 +7727,15 @@
       <c r="O57" s="78"/>
     </row>
     <row r="58" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="265"/>
+      <c r="A58" s="267"/>
       <c r="B58" s="198" t="s">
         <v>155</v>
       </c>
-      <c r="C58" s="269" t="s">
+      <c r="C58" s="271" t="s">
         <v>149</v>
       </c>
-      <c r="D58" s="270"/>
-      <c r="E58" s="271"/>
+      <c r="D58" s="272"/>
+      <c r="E58" s="273"/>
       <c r="F58" s="167" t="s">
         <v>71</v>
       </c>
@@ -7764,17 +7764,17 @@
       <c r="O58" s="78"/>
     </row>
     <row r="59" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="263">
+      <c r="A59" s="265">
         <v>31</v>
       </c>
       <c r="B59" s="156" t="s">
         <v>156</v>
       </c>
-      <c r="C59" s="269" t="s">
+      <c r="C59" s="271" t="s">
         <v>42</v>
       </c>
-      <c r="D59" s="270"/>
-      <c r="E59" s="271"/>
+      <c r="D59" s="272"/>
+      <c r="E59" s="273"/>
       <c r="F59" s="167" t="s">
         <v>71</v>
       </c>
@@ -7805,15 +7805,15 @@
       <c r="O59" s="78"/>
     </row>
     <row r="60" spans="1:15" s="79" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="265"/>
+      <c r="A60" s="267"/>
       <c r="B60" s="198" t="s">
         <v>158</v>
       </c>
-      <c r="C60" s="269" t="s">
+      <c r="C60" s="271" t="s">
         <v>54</v>
       </c>
-      <c r="D60" s="270"/>
-      <c r="E60" s="271"/>
+      <c r="D60" s="272"/>
+      <c r="E60" s="273"/>
       <c r="F60" s="167" t="s">
         <v>71</v>
       </c>
@@ -7841,17 +7841,17 @@
       <c r="N60" s="136"/>
     </row>
     <row r="61" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="263">
+      <c r="A61" s="265">
         <v>32</v>
       </c>
       <c r="B61" s="198" t="s">
         <v>159</v>
       </c>
-      <c r="C61" s="269" t="s">
+      <c r="C61" s="271" t="s">
         <v>160</v>
       </c>
-      <c r="D61" s="270"/>
-      <c r="E61" s="271"/>
+      <c r="D61" s="272"/>
+      <c r="E61" s="273"/>
       <c r="F61" s="167" t="s">
         <v>71</v>
       </c>
@@ -7882,15 +7882,15 @@
       <c r="O61" s="78"/>
     </row>
     <row r="62" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="265"/>
+      <c r="A62" s="267"/>
       <c r="B62" s="198" t="s">
         <v>161</v>
       </c>
-      <c r="C62" s="269" t="s">
+      <c r="C62" s="271" t="s">
         <v>162</v>
       </c>
-      <c r="D62" s="270"/>
-      <c r="E62" s="271"/>
+      <c r="D62" s="272"/>
+      <c r="E62" s="273"/>
       <c r="F62" s="167" t="s">
         <v>71</v>
       </c>
@@ -7925,11 +7925,11 @@
       <c r="B63" s="198" t="s">
         <v>163</v>
       </c>
-      <c r="C63" s="269" t="s">
+      <c r="C63" s="271" t="s">
         <v>164</v>
       </c>
-      <c r="D63" s="270"/>
-      <c r="E63" s="271"/>
+      <c r="D63" s="272"/>
+      <c r="E63" s="273"/>
       <c r="F63" s="167" t="s">
         <v>71</v>
       </c>
@@ -7966,11 +7966,11 @@
       <c r="B64" s="198" t="s">
         <v>167</v>
       </c>
-      <c r="C64" s="269" t="s">
+      <c r="C64" s="271" t="s">
         <v>164</v>
       </c>
-      <c r="D64" s="270"/>
-      <c r="E64" s="271"/>
+      <c r="D64" s="272"/>
+      <c r="E64" s="273"/>
       <c r="F64" s="167" t="s">
         <v>71</v>
       </c>
@@ -8001,17 +8001,17 @@
       <c r="O64" s="78"/>
     </row>
     <row r="65" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="263">
+      <c r="A65" s="265">
         <v>35</v>
       </c>
-      <c r="B65" s="307" t="s">
+      <c r="B65" s="312" t="s">
         <v>168</v>
       </c>
-      <c r="C65" s="269" t="s">
+      <c r="C65" s="271" t="s">
         <v>169</v>
       </c>
-      <c r="D65" s="270"/>
-      <c r="E65" s="271"/>
+      <c r="D65" s="272"/>
+      <c r="E65" s="273"/>
       <c r="F65" s="167" t="s">
         <v>71</v>
       </c>
@@ -8036,19 +8036,19 @@
       <c r="M65" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N65" s="317" t="s">
+      <c r="N65" s="322" t="s">
         <v>48</v>
       </c>
       <c r="O65" s="78"/>
     </row>
     <row r="66" spans="1:15" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="264"/>
-      <c r="B66" s="308"/>
-      <c r="C66" s="269" t="s">
+      <c r="A66" s="266"/>
+      <c r="B66" s="313"/>
+      <c r="C66" s="271" t="s">
         <v>60</v>
       </c>
-      <c r="D66" s="270"/>
-      <c r="E66" s="271"/>
+      <c r="D66" s="272"/>
+      <c r="E66" s="273"/>
       <c r="F66" s="167" t="s">
         <v>65</v>
       </c>
@@ -8073,16 +8073,16 @@
       <c r="M66" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N66" s="318"/>
+      <c r="N66" s="323"/>
     </row>
     <row r="67" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="265"/>
-      <c r="B67" s="309"/>
-      <c r="C67" s="269" t="s">
+      <c r="A67" s="267"/>
+      <c r="B67" s="314"/>
+      <c r="C67" s="271" t="s">
         <v>61</v>
       </c>
-      <c r="D67" s="270"/>
-      <c r="E67" s="271"/>
+      <c r="D67" s="272"/>
+      <c r="E67" s="273"/>
       <c r="F67" s="167" t="s">
         <v>65</v>
       </c>
@@ -8117,11 +8117,11 @@
       <c r="B68" s="162" t="s">
         <v>171</v>
       </c>
-      <c r="C68" s="269" t="s">
+      <c r="C68" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="D68" s="270"/>
-      <c r="E68" s="271"/>
+      <c r="D68" s="272"/>
+      <c r="E68" s="273"/>
       <c r="F68" s="167" t="s">
         <v>71</v>
       </c>
@@ -8158,11 +8158,11 @@
       <c r="B69" s="162" t="s">
         <v>173</v>
       </c>
-      <c r="C69" s="269" t="s">
+      <c r="C69" s="271" t="s">
         <v>251</v>
       </c>
-      <c r="D69" s="270"/>
-      <c r="E69" s="271"/>
+      <c r="D69" s="272"/>
+      <c r="E69" s="273"/>
       <c r="F69" s="167" t="s">
         <v>71</v>
       </c>
@@ -8192,17 +8192,17 @@
       </c>
     </row>
     <row r="70" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="263">
+      <c r="A70" s="265">
         <v>38</v>
       </c>
       <c r="B70" s="156" t="s">
         <v>174</v>
       </c>
-      <c r="C70" s="269" t="s">
+      <c r="C70" s="271" t="s">
         <v>43</v>
       </c>
-      <c r="D70" s="270"/>
-      <c r="E70" s="271"/>
+      <c r="D70" s="272"/>
+      <c r="E70" s="273"/>
       <c r="F70" s="167" t="s">
         <v>71</v>
       </c>
@@ -8227,21 +8227,21 @@
       <c r="M70" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N70" s="317" t="s">
+      <c r="N70" s="322" t="s">
         <v>45</v>
       </c>
       <c r="O70" s="78"/>
     </row>
     <row r="71" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="265"/>
+      <c r="A71" s="267"/>
       <c r="B71" s="198" t="s">
         <v>175</v>
       </c>
-      <c r="C71" s="269" t="s">
+      <c r="C71" s="271" t="s">
         <v>55</v>
       </c>
-      <c r="D71" s="270"/>
-      <c r="E71" s="271"/>
+      <c r="D71" s="272"/>
+      <c r="E71" s="273"/>
       <c r="F71" s="167" t="s">
         <v>71</v>
       </c>
@@ -8266,21 +8266,21 @@
       <c r="M71" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N71" s="318"/>
+      <c r="N71" s="323"/>
       <c r="O71" s="78"/>
     </row>
     <row r="72" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="263">
+      <c r="A72" s="265">
         <v>39</v>
       </c>
       <c r="B72" s="198" t="s">
         <v>176</v>
       </c>
-      <c r="C72" s="269" t="s">
+      <c r="C72" s="271" t="s">
         <v>204</v>
       </c>
-      <c r="D72" s="270"/>
-      <c r="E72" s="271"/>
+      <c r="D72" s="272"/>
+      <c r="E72" s="273"/>
       <c r="F72" s="167" t="s">
         <v>71</v>
       </c>
@@ -8305,21 +8305,21 @@
       <c r="M72" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N72" s="317" t="s">
+      <c r="N72" s="322" t="s">
         <v>177</v>
       </c>
       <c r="O72" s="78"/>
     </row>
     <row r="73" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="265"/>
+      <c r="A73" s="267"/>
       <c r="B73" s="198" t="s">
         <v>178</v>
       </c>
-      <c r="C73" s="269" t="s">
+      <c r="C73" s="271" t="s">
         <v>205</v>
       </c>
-      <c r="D73" s="270"/>
-      <c r="E73" s="271"/>
+      <c r="D73" s="272"/>
+      <c r="E73" s="273"/>
       <c r="F73" s="167" t="s">
         <v>71</v>
       </c>
@@ -8344,7 +8344,7 @@
       <c r="M73" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N73" s="318"/>
+      <c r="N73" s="323"/>
       <c r="O73" s="78"/>
     </row>
     <row r="74" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8354,11 +8354,11 @@
       <c r="B74" s="198" t="s">
         <v>214</v>
       </c>
-      <c r="C74" s="269" t="s">
+      <c r="C74" s="271" t="s">
         <v>64</v>
       </c>
-      <c r="D74" s="270"/>
-      <c r="E74" s="271"/>
+      <c r="D74" s="272"/>
+      <c r="E74" s="273"/>
       <c r="F74" s="167" t="s">
         <v>71</v>
       </c>
@@ -8395,11 +8395,11 @@
       <c r="B75" s="198" t="s">
         <v>215</v>
       </c>
-      <c r="C75" s="269" t="s">
+      <c r="C75" s="271" t="s">
         <v>64</v>
       </c>
-      <c r="D75" s="270"/>
-      <c r="E75" s="271"/>
+      <c r="D75" s="272"/>
+      <c r="E75" s="273"/>
       <c r="F75" s="167" t="s">
         <v>71</v>
       </c>
@@ -8436,11 +8436,11 @@
       <c r="B76" s="198" t="s">
         <v>179</v>
       </c>
-      <c r="C76" s="269" t="s">
+      <c r="C76" s="271" t="s">
         <v>180</v>
       </c>
-      <c r="D76" s="270"/>
-      <c r="E76" s="271"/>
+      <c r="D76" s="272"/>
+      <c r="E76" s="273"/>
       <c r="F76" s="167" t="s">
         <v>71</v>
       </c>
@@ -8477,11 +8477,11 @@
       <c r="B77" s="198" t="s">
         <v>181</v>
       </c>
-      <c r="C77" s="269" t="s">
+      <c r="C77" s="271" t="s">
         <v>180</v>
       </c>
-      <c r="D77" s="270"/>
-      <c r="E77" s="271"/>
+      <c r="D77" s="272"/>
+      <c r="E77" s="273"/>
       <c r="F77" s="167" t="s">
         <v>71</v>
       </c>
@@ -8517,11 +8517,11 @@
       <c r="B78" s="198" t="s">
         <v>182</v>
       </c>
-      <c r="C78" s="269" t="s">
+      <c r="C78" s="271" t="s">
         <v>41</v>
       </c>
-      <c r="D78" s="270"/>
-      <c r="E78" s="271"/>
+      <c r="D78" s="272"/>
+      <c r="E78" s="273"/>
       <c r="F78" s="167" t="s">
         <v>71</v>
       </c>
@@ -8546,7 +8546,7 @@
       <c r="M78" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N78" s="317" t="s">
+      <c r="N78" s="322" t="s">
         <v>177</v>
       </c>
       <c r="O78" s="78"/>
@@ -8558,11 +8558,11 @@
       <c r="B79" s="198" t="s">
         <v>183</v>
       </c>
-      <c r="C79" s="269" t="s">
+      <c r="C79" s="271" t="s">
         <v>41</v>
       </c>
-      <c r="D79" s="270"/>
-      <c r="E79" s="271"/>
+      <c r="D79" s="272"/>
+      <c r="E79" s="273"/>
       <c r="F79" s="167" t="s">
         <v>71</v>
       </c>
@@ -8587,7 +8587,7 @@
       <c r="M79" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N79" s="318"/>
+      <c r="N79" s="323"/>
       <c r="O79" s="78"/>
     </row>
     <row r="80" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8597,11 +8597,11 @@
       <c r="B80" s="198" t="s">
         <v>184</v>
       </c>
-      <c r="C80" s="269" t="s">
+      <c r="C80" s="271" t="s">
         <v>53</v>
       </c>
-      <c r="D80" s="270"/>
-      <c r="E80" s="271"/>
+      <c r="D80" s="272"/>
+      <c r="E80" s="273"/>
       <c r="F80" s="167" t="s">
         <v>71</v>
       </c>
@@ -8636,11 +8636,11 @@
       <c r="B81" s="198" t="s">
         <v>185</v>
       </c>
-      <c r="C81" s="269" t="s">
+      <c r="C81" s="271" t="s">
         <v>53</v>
       </c>
-      <c r="D81" s="270"/>
-      <c r="E81" s="271"/>
+      <c r="D81" s="272"/>
+      <c r="E81" s="273"/>
       <c r="F81" s="167" t="s">
         <v>71</v>
       </c>
@@ -8675,11 +8675,11 @@
       <c r="B82" s="198" t="s">
         <v>186</v>
       </c>
-      <c r="C82" s="269" t="s">
+      <c r="C82" s="271" t="s">
         <v>187</v>
       </c>
-      <c r="D82" s="270"/>
-      <c r="E82" s="271"/>
+      <c r="D82" s="272"/>
+      <c r="E82" s="273"/>
       <c r="F82" s="167" t="s">
         <v>71</v>
       </c>
@@ -8704,7 +8704,7 @@
       <c r="M82" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N82" s="317" t="s">
+      <c r="N82" s="322" t="s">
         <v>177</v>
       </c>
       <c r="O82" s="78"/>
@@ -8716,11 +8716,11 @@
       <c r="B83" s="198" t="s">
         <v>188</v>
       </c>
-      <c r="C83" s="269" t="s">
+      <c r="C83" s="271" t="s">
         <v>187</v>
       </c>
-      <c r="D83" s="270"/>
-      <c r="E83" s="271"/>
+      <c r="D83" s="272"/>
+      <c r="E83" s="273"/>
       <c r="F83" s="167" t="s">
         <v>71</v>
       </c>
@@ -8745,7 +8745,7 @@
       <c r="M83" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="N83" s="318"/>
+      <c r="N83" s="323"/>
       <c r="O83" s="78"/>
     </row>
     <row r="84" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8755,11 +8755,11 @@
       <c r="B84" s="198" t="s">
         <v>189</v>
       </c>
-      <c r="C84" s="269" t="s">
+      <c r="C84" s="271" t="s">
         <v>190</v>
       </c>
-      <c r="D84" s="270"/>
-      <c r="E84" s="271"/>
+      <c r="D84" s="272"/>
+      <c r="E84" s="273"/>
       <c r="F84" s="167" t="s">
         <v>71</v>
       </c>
@@ -8794,11 +8794,11 @@
       <c r="B85" s="198" t="s">
         <v>191</v>
       </c>
-      <c r="C85" s="269" t="s">
+      <c r="C85" s="271" t="s">
         <v>190</v>
       </c>
-      <c r="D85" s="270"/>
-      <c r="E85" s="271"/>
+      <c r="D85" s="272"/>
+      <c r="E85" s="273"/>
       <c r="F85" s="167" t="s">
         <v>71</v>
       </c>
@@ -8833,11 +8833,11 @@
       <c r="B86" s="158" t="s">
         <v>192</v>
       </c>
-      <c r="C86" s="269" t="s">
+      <c r="C86" s="271" t="s">
         <v>193</v>
       </c>
-      <c r="D86" s="270"/>
-      <c r="E86" s="271"/>
+      <c r="D86" s="272"/>
+      <c r="E86" s="273"/>
       <c r="F86" s="167" t="s">
         <v>71</v>
       </c>
@@ -8874,11 +8874,11 @@
       <c r="B87" s="198" t="s">
         <v>286</v>
       </c>
-      <c r="C87" s="266" t="s">
+      <c r="C87" s="268" t="s">
         <v>50</v>
       </c>
-      <c r="D87" s="267"/>
-      <c r="E87" s="268"/>
+      <c r="D87" s="269"/>
+      <c r="E87" s="270"/>
       <c r="F87" s="167" t="s">
         <v>71</v>
       </c>
@@ -8915,11 +8915,11 @@
       <c r="B88" s="167" t="s">
         <v>287</v>
       </c>
-      <c r="C88" s="266" t="s">
+      <c r="C88" s="268" t="s">
         <v>51</v>
       </c>
-      <c r="D88" s="267"/>
-      <c r="E88" s="268"/>
+      <c r="D88" s="269"/>
+      <c r="E88" s="270"/>
       <c r="F88" s="167" t="s">
         <v>71</v>
       </c>
@@ -8949,17 +8949,17 @@
       </c>
     </row>
     <row r="89" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="263">
+      <c r="A89" s="265">
         <v>55</v>
       </c>
-      <c r="B89" s="297" t="s">
+      <c r="B89" s="302" t="s">
         <v>283</v>
       </c>
-      <c r="C89" s="266" t="s">
+      <c r="C89" s="268" t="s">
         <v>78</v>
       </c>
-      <c r="D89" s="267"/>
-      <c r="E89" s="268"/>
+      <c r="D89" s="269"/>
+      <c r="E89" s="270"/>
       <c r="F89" s="167" t="s">
         <v>79</v>
       </c>
@@ -8988,13 +8988,13 @@
       <c r="O89" s="78"/>
     </row>
     <row r="90" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="264"/>
-      <c r="B90" s="298"/>
-      <c r="C90" s="266" t="s">
+      <c r="A90" s="266"/>
+      <c r="B90" s="303"/>
+      <c r="C90" s="268" t="s">
         <v>217</v>
       </c>
-      <c r="D90" s="267"/>
-      <c r="E90" s="268"/>
+      <c r="D90" s="269"/>
+      <c r="E90" s="270"/>
       <c r="F90" s="167" t="s">
         <v>79</v>
       </c>
@@ -9025,13 +9025,13 @@
       <c r="O90" s="78"/>
     </row>
     <row r="91" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="264"/>
-      <c r="B91" s="298"/>
-      <c r="C91" s="266" t="s">
+      <c r="A91" s="266"/>
+      <c r="B91" s="303"/>
+      <c r="C91" s="268" t="s">
         <v>218</v>
       </c>
-      <c r="D91" s="267"/>
-      <c r="E91" s="268"/>
+      <c r="D91" s="269"/>
+      <c r="E91" s="270"/>
       <c r="F91" s="167" t="s">
         <v>79</v>
       </c>
@@ -9062,13 +9062,13 @@
       <c r="O91" s="78"/>
     </row>
     <row r="92" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="264"/>
-      <c r="B92" s="298"/>
-      <c r="C92" s="266" t="s">
+      <c r="A92" s="266"/>
+      <c r="B92" s="303"/>
+      <c r="C92" s="268" t="s">
         <v>236</v>
       </c>
-      <c r="D92" s="267"/>
-      <c r="E92" s="268"/>
+      <c r="D92" s="269"/>
+      <c r="E92" s="270"/>
       <c r="F92" s="167" t="s">
         <v>79</v>
       </c>
@@ -9099,13 +9099,13 @@
       <c r="O92" s="78"/>
     </row>
     <row r="93" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="264"/>
-      <c r="B93" s="298"/>
-      <c r="C93" s="266" t="s">
+      <c r="A93" s="266"/>
+      <c r="B93" s="303"/>
+      <c r="C93" s="268" t="s">
         <v>237</v>
       </c>
-      <c r="D93" s="267"/>
-      <c r="E93" s="268"/>
+      <c r="D93" s="269"/>
+      <c r="E93" s="270"/>
       <c r="F93" s="167" t="s">
         <v>79</v>
       </c>
@@ -9136,13 +9136,13 @@
       <c r="O93" s="78"/>
     </row>
     <row r="94" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="264"/>
-      <c r="B94" s="298"/>
-      <c r="C94" s="266" t="s">
+      <c r="A94" s="266"/>
+      <c r="B94" s="303"/>
+      <c r="C94" s="268" t="s">
         <v>220</v>
       </c>
-      <c r="D94" s="267"/>
-      <c r="E94" s="268"/>
+      <c r="D94" s="269"/>
+      <c r="E94" s="270"/>
       <c r="F94" s="167" t="s">
         <v>79</v>
       </c>
@@ -9173,13 +9173,13 @@
       <c r="O94" s="78"/>
     </row>
     <row r="95" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="264"/>
-      <c r="B95" s="298"/>
-      <c r="C95" s="266" t="s">
+      <c r="A95" s="266"/>
+      <c r="B95" s="303"/>
+      <c r="C95" s="268" t="s">
         <v>221</v>
       </c>
-      <c r="D95" s="267"/>
-      <c r="E95" s="268"/>
+      <c r="D95" s="269"/>
+      <c r="E95" s="270"/>
       <c r="F95" s="167" t="s">
         <v>79</v>
       </c>
@@ -9210,13 +9210,13 @@
       <c r="O95" s="78"/>
     </row>
     <row r="96" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="264"/>
-      <c r="B96" s="298"/>
-      <c r="C96" s="266" t="s">
+      <c r="A96" s="266"/>
+      <c r="B96" s="303"/>
+      <c r="C96" s="268" t="s">
         <v>222</v>
       </c>
-      <c r="D96" s="267"/>
-      <c r="E96" s="268"/>
+      <c r="D96" s="269"/>
+      <c r="E96" s="270"/>
       <c r="F96" s="167" t="s">
         <v>79</v>
       </c>
@@ -9247,13 +9247,13 @@
       <c r="O96" s="78"/>
     </row>
     <row r="97" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="264"/>
-      <c r="B97" s="298"/>
-      <c r="C97" s="266" t="s">
+      <c r="A97" s="266"/>
+      <c r="B97" s="303"/>
+      <c r="C97" s="268" t="s">
         <v>223</v>
       </c>
-      <c r="D97" s="267"/>
-      <c r="E97" s="268"/>
+      <c r="D97" s="269"/>
+      <c r="E97" s="270"/>
       <c r="F97" s="167" t="s">
         <v>79</v>
       </c>
@@ -9284,13 +9284,13 @@
       <c r="O97" s="78"/>
     </row>
     <row r="98" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="264"/>
-      <c r="B98" s="298"/>
-      <c r="C98" s="266" t="s">
+      <c r="A98" s="266"/>
+      <c r="B98" s="303"/>
+      <c r="C98" s="268" t="s">
         <v>224</v>
       </c>
-      <c r="D98" s="267"/>
-      <c r="E98" s="268"/>
+      <c r="D98" s="269"/>
+      <c r="E98" s="270"/>
       <c r="F98" s="167" t="s">
         <v>79</v>
       </c>
@@ -9321,13 +9321,13 @@
       <c r="O98" s="78"/>
     </row>
     <row r="99" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="264"/>
-      <c r="B99" s="298"/>
-      <c r="C99" s="266" t="s">
+      <c r="A99" s="266"/>
+      <c r="B99" s="303"/>
+      <c r="C99" s="268" t="s">
         <v>225</v>
       </c>
-      <c r="D99" s="267"/>
-      <c r="E99" s="268"/>
+      <c r="D99" s="269"/>
+      <c r="E99" s="270"/>
       <c r="F99" s="167" t="s">
         <v>79</v>
       </c>
@@ -9358,13 +9358,13 @@
       <c r="O99" s="78"/>
     </row>
     <row r="100" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="264"/>
-      <c r="B100" s="298"/>
-      <c r="C100" s="266" t="s">
+      <c r="A100" s="266"/>
+      <c r="B100" s="303"/>
+      <c r="C100" s="268" t="s">
         <v>226</v>
       </c>
-      <c r="D100" s="267"/>
-      <c r="E100" s="268"/>
+      <c r="D100" s="269"/>
+      <c r="E100" s="270"/>
       <c r="F100" s="167" t="s">
         <v>79</v>
       </c>
@@ -9395,13 +9395,13 @@
       <c r="O100" s="78"/>
     </row>
     <row r="101" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="264"/>
-      <c r="B101" s="298"/>
-      <c r="C101" s="266" t="s">
+      <c r="A101" s="266"/>
+      <c r="B101" s="303"/>
+      <c r="C101" s="268" t="s">
         <v>260</v>
       </c>
-      <c r="D101" s="267"/>
-      <c r="E101" s="268"/>
+      <c r="D101" s="269"/>
+      <c r="E101" s="270"/>
       <c r="F101" s="167" t="s">
         <v>79</v>
       </c>
@@ -9432,13 +9432,13 @@
       <c r="O101" s="78"/>
     </row>
     <row r="102" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="264"/>
-      <c r="B102" s="298"/>
-      <c r="C102" s="266" t="s">
+      <c r="A102" s="266"/>
+      <c r="B102" s="303"/>
+      <c r="C102" s="268" t="s">
         <v>227</v>
       </c>
-      <c r="D102" s="267"/>
-      <c r="E102" s="268"/>
+      <c r="D102" s="269"/>
+      <c r="E102" s="270"/>
       <c r="F102" s="167" t="s">
         <v>79</v>
       </c>
@@ -9469,13 +9469,13 @@
       <c r="O102" s="78"/>
     </row>
     <row r="103" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="264"/>
-      <c r="B103" s="298"/>
-      <c r="C103" s="266" t="s">
+      <c r="A103" s="266"/>
+      <c r="B103" s="303"/>
+      <c r="C103" s="268" t="s">
         <v>228</v>
       </c>
-      <c r="D103" s="267"/>
-      <c r="E103" s="268"/>
+      <c r="D103" s="269"/>
+      <c r="E103" s="270"/>
       <c r="F103" s="167" t="s">
         <v>79</v>
       </c>
@@ -9506,13 +9506,13 @@
       <c r="O103" s="78"/>
     </row>
     <row r="104" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="264"/>
-      <c r="B104" s="298"/>
-      <c r="C104" s="266" t="s">
+      <c r="A104" s="266"/>
+      <c r="B104" s="303"/>
+      <c r="C104" s="268" t="s">
         <v>44</v>
       </c>
-      <c r="D104" s="267"/>
-      <c r="E104" s="268"/>
+      <c r="D104" s="269"/>
+      <c r="E104" s="270"/>
       <c r="F104" s="167" t="s">
         <v>79</v>
       </c>
@@ -9543,13 +9543,13 @@
       <c r="O104" s="78"/>
     </row>
     <row r="105" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="264"/>
-      <c r="B105" s="298"/>
-      <c r="C105" s="266" t="s">
+      <c r="A105" s="266"/>
+      <c r="B105" s="303"/>
+      <c r="C105" s="268" t="s">
         <v>229</v>
       </c>
-      <c r="D105" s="267"/>
-      <c r="E105" s="268"/>
+      <c r="D105" s="269"/>
+      <c r="E105" s="270"/>
       <c r="F105" s="167" t="s">
         <v>79</v>
       </c>
@@ -9580,13 +9580,13 @@
       <c r="O105" s="78"/>
     </row>
     <row r="106" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="264"/>
-      <c r="B106" s="298"/>
-      <c r="C106" s="266" t="s">
+      <c r="A106" s="266"/>
+      <c r="B106" s="303"/>
+      <c r="C106" s="268" t="s">
         <v>238</v>
       </c>
-      <c r="D106" s="267"/>
-      <c r="E106" s="268"/>
+      <c r="D106" s="269"/>
+      <c r="E106" s="270"/>
       <c r="F106" s="167" t="s">
         <v>79</v>
       </c>
@@ -9617,13 +9617,13 @@
       <c r="O106" s="78"/>
     </row>
     <row r="107" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="264"/>
-      <c r="B107" s="298"/>
-      <c r="C107" s="266" t="s">
+      <c r="A107" s="266"/>
+      <c r="B107" s="303"/>
+      <c r="C107" s="268" t="s">
         <v>230</v>
       </c>
-      <c r="D107" s="267"/>
-      <c r="E107" s="268"/>
+      <c r="D107" s="269"/>
+      <c r="E107" s="270"/>
       <c r="F107" s="167" t="s">
         <v>79</v>
       </c>
@@ -9654,13 +9654,13 @@
       <c r="O107" s="78"/>
     </row>
     <row r="108" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="264"/>
-      <c r="B108" s="298"/>
-      <c r="C108" s="266" t="s">
+      <c r="A108" s="266"/>
+      <c r="B108" s="303"/>
+      <c r="C108" s="268" t="s">
         <v>230</v>
       </c>
-      <c r="D108" s="267"/>
-      <c r="E108" s="268"/>
+      <c r="D108" s="269"/>
+      <c r="E108" s="270"/>
       <c r="F108" s="167" t="s">
         <v>79</v>
       </c>
@@ -9691,13 +9691,13 @@
       <c r="O108" s="78"/>
     </row>
     <row r="109" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="264"/>
-      <c r="B109" s="298"/>
-      <c r="C109" s="266" t="s">
+      <c r="A109" s="266"/>
+      <c r="B109" s="303"/>
+      <c r="C109" s="268" t="s">
         <v>230</v>
       </c>
-      <c r="D109" s="267"/>
-      <c r="E109" s="268"/>
+      <c r="D109" s="269"/>
+      <c r="E109" s="270"/>
       <c r="F109" s="167" t="s">
         <v>79</v>
       </c>
@@ -9728,13 +9728,13 @@
       <c r="O109" s="78"/>
     </row>
     <row r="110" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="264"/>
-      <c r="B110" s="298"/>
-      <c r="C110" s="266" t="s">
+      <c r="A110" s="266"/>
+      <c r="B110" s="303"/>
+      <c r="C110" s="268" t="s">
         <v>231</v>
       </c>
-      <c r="D110" s="267"/>
-      <c r="E110" s="268"/>
+      <c r="D110" s="269"/>
+      <c r="E110" s="270"/>
       <c r="F110" s="167" t="s">
         <v>79</v>
       </c>
@@ -9765,13 +9765,13 @@
       <c r="O110" s="78"/>
     </row>
     <row r="111" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="264"/>
-      <c r="B111" s="298"/>
-      <c r="C111" s="266" t="s">
+      <c r="A111" s="266"/>
+      <c r="B111" s="303"/>
+      <c r="C111" s="268" t="s">
         <v>248</v>
       </c>
-      <c r="D111" s="267"/>
-      <c r="E111" s="268"/>
+      <c r="D111" s="269"/>
+      <c r="E111" s="270"/>
       <c r="F111" s="167" t="s">
         <v>79</v>
       </c>
@@ -9802,13 +9802,13 @@
       <c r="O111" s="78"/>
     </row>
     <row r="112" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="264"/>
-      <c r="B112" s="298"/>
-      <c r="C112" s="266" t="s">
+      <c r="A112" s="266"/>
+      <c r="B112" s="303"/>
+      <c r="C112" s="268" t="s">
         <v>261</v>
       </c>
-      <c r="D112" s="267"/>
-      <c r="E112" s="268"/>
+      <c r="D112" s="269"/>
+      <c r="E112" s="270"/>
       <c r="F112" s="163" t="s">
         <v>87</v>
       </c>
@@ -9839,13 +9839,13 @@
       <c r="O112" s="78"/>
     </row>
     <row r="113" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="264"/>
-      <c r="B113" s="298"/>
-      <c r="C113" s="266" t="s">
+      <c r="A113" s="266"/>
+      <c r="B113" s="303"/>
+      <c r="C113" s="268" t="s">
         <v>200</v>
       </c>
-      <c r="D113" s="267"/>
-      <c r="E113" s="268"/>
+      <c r="D113" s="269"/>
+      <c r="E113" s="270"/>
       <c r="F113" s="167" t="s">
         <v>78</v>
       </c>
@@ -9876,13 +9876,13 @@
       <c r="O113" s="78"/>
     </row>
     <row r="114" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="264"/>
-      <c r="B114" s="298"/>
-      <c r="C114" s="269" t="s">
+      <c r="A114" s="266"/>
+      <c r="B114" s="303"/>
+      <c r="C114" s="271" t="s">
         <v>194</v>
       </c>
-      <c r="D114" s="270"/>
-      <c r="E114" s="271"/>
+      <c r="D114" s="272"/>
+      <c r="E114" s="273"/>
       <c r="F114" s="167" t="s">
         <v>232</v>
       </c>
@@ -9913,13 +9913,13 @@
       <c r="O114" s="78"/>
     </row>
     <row r="115" spans="1:15" s="171" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="264"/>
-      <c r="B115" s="298"/>
-      <c r="C115" s="319" t="s">
+      <c r="A115" s="266"/>
+      <c r="B115" s="303"/>
+      <c r="C115" s="324" t="s">
         <v>263</v>
       </c>
-      <c r="D115" s="320"/>
-      <c r="E115" s="321"/>
+      <c r="D115" s="325"/>
+      <c r="E115" s="326"/>
       <c r="F115" s="203" t="s">
         <v>78</v>
       </c>
@@ -9949,13 +9949,13 @@
       </c>
     </row>
     <row r="116" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="265"/>
-      <c r="B116" s="299"/>
-      <c r="C116" s="266" t="s">
+      <c r="A116" s="267"/>
+      <c r="B116" s="304"/>
+      <c r="C116" s="268" t="s">
         <v>76</v>
       </c>
-      <c r="D116" s="267"/>
-      <c r="E116" s="268"/>
+      <c r="D116" s="269"/>
+      <c r="E116" s="270"/>
       <c r="F116" s="167" t="s">
         <v>263</v>
       </c>
@@ -9986,17 +9986,17 @@
       <c r="O116" s="78"/>
     </row>
     <row r="117" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="263">
+      <c r="A117" s="265">
         <v>56</v>
       </c>
-      <c r="B117" s="297" t="s">
+      <c r="B117" s="302" t="s">
         <v>284</v>
       </c>
-      <c r="C117" s="266" t="s">
+      <c r="C117" s="268" t="s">
         <v>66</v>
       </c>
-      <c r="D117" s="267"/>
-      <c r="E117" s="268"/>
+      <c r="D117" s="269"/>
+      <c r="E117" s="270"/>
       <c r="F117" s="167" t="s">
         <v>76</v>
       </c>
@@ -10027,13 +10027,13 @@
       <c r="O117" s="78"/>
     </row>
     <row r="118" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="264"/>
-      <c r="B118" s="298"/>
-      <c r="C118" s="266" t="s">
+      <c r="A118" s="266"/>
+      <c r="B118" s="303"/>
+      <c r="C118" s="268" t="s">
         <v>67</v>
       </c>
-      <c r="D118" s="267"/>
-      <c r="E118" s="268"/>
+      <c r="D118" s="269"/>
+      <c r="E118" s="270"/>
       <c r="F118" s="167" t="s">
         <v>76</v>
       </c>
@@ -10064,13 +10064,13 @@
       <c r="O118" s="78"/>
     </row>
     <row r="119" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="264"/>
-      <c r="B119" s="298"/>
-      <c r="C119" s="266" t="s">
+      <c r="A119" s="266"/>
+      <c r="B119" s="303"/>
+      <c r="C119" s="268" t="s">
         <v>68</v>
       </c>
-      <c r="D119" s="267"/>
-      <c r="E119" s="268"/>
+      <c r="D119" s="269"/>
+      <c r="E119" s="270"/>
       <c r="F119" s="167" t="s">
         <v>76</v>
       </c>
@@ -10101,13 +10101,13 @@
       <c r="O119" s="78"/>
     </row>
     <row r="120" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="265"/>
-      <c r="B120" s="299"/>
-      <c r="C120" s="266" t="s">
+      <c r="A120" s="267"/>
+      <c r="B120" s="304"/>
+      <c r="C120" s="268" t="s">
         <v>69</v>
       </c>
-      <c r="D120" s="267"/>
-      <c r="E120" s="268"/>
+      <c r="D120" s="269"/>
+      <c r="E120" s="270"/>
       <c r="F120" s="167" t="s">
         <v>76</v>
       </c>
@@ -10138,17 +10138,17 @@
       <c r="O120" s="78"/>
     </row>
     <row r="121" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="263">
+      <c r="A121" s="265">
         <v>57</v>
       </c>
-      <c r="B121" s="297" t="s">
+      <c r="B121" s="302" t="s">
         <v>285</v>
       </c>
-      <c r="C121" s="269" t="s">
+      <c r="C121" s="271" t="s">
         <v>85</v>
       </c>
-      <c r="D121" s="270"/>
-      <c r="E121" s="271"/>
+      <c r="D121" s="272"/>
+      <c r="E121" s="273"/>
       <c r="F121" s="167" t="s">
         <v>71</v>
       </c>
@@ -10179,13 +10179,13 @@
       <c r="O121" s="78"/>
     </row>
     <row r="122" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="264"/>
-      <c r="B122" s="298"/>
-      <c r="C122" s="269" t="s">
+      <c r="A122" s="266"/>
+      <c r="B122" s="303"/>
+      <c r="C122" s="271" t="s">
         <v>209</v>
       </c>
-      <c r="D122" s="270"/>
-      <c r="E122" s="271"/>
+      <c r="D122" s="272"/>
+      <c r="E122" s="273"/>
       <c r="F122" s="167" t="s">
         <v>73</v>
       </c>
@@ -10216,13 +10216,13 @@
       <c r="O122" s="78"/>
     </row>
     <row r="123" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="264"/>
-      <c r="B123" s="298"/>
-      <c r="C123" s="269" t="s">
+      <c r="A123" s="266"/>
+      <c r="B123" s="303"/>
+      <c r="C123" s="271" t="s">
         <v>210</v>
       </c>
-      <c r="D123" s="270"/>
-      <c r="E123" s="271"/>
+      <c r="D123" s="272"/>
+      <c r="E123" s="273"/>
       <c r="F123" s="167" t="s">
         <v>73</v>
       </c>
@@ -10253,13 +10253,13 @@
       <c r="O123" s="78"/>
     </row>
     <row r="124" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="264"/>
-      <c r="B124" s="298"/>
-      <c r="C124" s="269" t="s">
+      <c r="A124" s="266"/>
+      <c r="B124" s="303"/>
+      <c r="C124" s="271" t="s">
         <v>211</v>
       </c>
-      <c r="D124" s="270"/>
-      <c r="E124" s="271"/>
+      <c r="D124" s="272"/>
+      <c r="E124" s="273"/>
       <c r="F124" s="167" t="s">
         <v>73</v>
       </c>
@@ -10290,13 +10290,13 @@
       <c r="O124" s="78"/>
     </row>
     <row r="125" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="264"/>
-      <c r="B125" s="298"/>
-      <c r="C125" s="269" t="s">
+      <c r="A125" s="266"/>
+      <c r="B125" s="303"/>
+      <c r="C125" s="271" t="s">
         <v>62</v>
       </c>
-      <c r="D125" s="270"/>
-      <c r="E125" s="271"/>
+      <c r="D125" s="272"/>
+      <c r="E125" s="273"/>
       <c r="F125" s="167" t="s">
         <v>73</v>
       </c>
@@ -10327,13 +10327,13 @@
       <c r="O125" s="78"/>
     </row>
     <row r="126" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="264"/>
-      <c r="B126" s="298"/>
-      <c r="C126" s="269" t="s">
+      <c r="A126" s="266"/>
+      <c r="B126" s="303"/>
+      <c r="C126" s="271" t="s">
         <v>63</v>
       </c>
-      <c r="D126" s="270"/>
-      <c r="E126" s="271"/>
+      <c r="D126" s="272"/>
+      <c r="E126" s="273"/>
       <c r="F126" s="167" t="s">
         <v>73</v>
       </c>
@@ -10364,13 +10364,13 @@
       <c r="O126" s="78"/>
     </row>
     <row r="127" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="264"/>
-      <c r="B127" s="298"/>
-      <c r="C127" s="269" t="s">
+      <c r="A127" s="266"/>
+      <c r="B127" s="303"/>
+      <c r="C127" s="271" t="s">
         <v>197</v>
       </c>
-      <c r="D127" s="270"/>
-      <c r="E127" s="271"/>
+      <c r="D127" s="272"/>
+      <c r="E127" s="273"/>
       <c r="F127" s="167" t="s">
         <v>73</v>
       </c>
@@ -10401,13 +10401,13 @@
       <c r="O127" s="78"/>
     </row>
     <row r="128" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="264"/>
-      <c r="B128" s="298"/>
-      <c r="C128" s="269" t="s">
+      <c r="A128" s="266"/>
+      <c r="B128" s="303"/>
+      <c r="C128" s="271" t="s">
         <v>198</v>
       </c>
-      <c r="D128" s="270"/>
-      <c r="E128" s="271"/>
+      <c r="D128" s="272"/>
+      <c r="E128" s="273"/>
       <c r="F128" s="167" t="s">
         <v>73</v>
       </c>
@@ -10438,13 +10438,13 @@
       <c r="O128" s="78"/>
     </row>
     <row r="129" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="264"/>
-      <c r="B129" s="298"/>
-      <c r="C129" s="269" t="s">
+      <c r="A129" s="266"/>
+      <c r="B129" s="303"/>
+      <c r="C129" s="271" t="s">
         <v>208</v>
       </c>
-      <c r="D129" s="270"/>
-      <c r="E129" s="271"/>
+      <c r="D129" s="272"/>
+      <c r="E129" s="273"/>
       <c r="F129" s="167" t="s">
         <v>73</v>
       </c>
@@ -10475,13 +10475,13 @@
       <c r="O129" s="78"/>
     </row>
     <row r="130" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="264"/>
-      <c r="B130" s="298"/>
-      <c r="C130" s="269" t="s">
+      <c r="A130" s="266"/>
+      <c r="B130" s="303"/>
+      <c r="C130" s="271" t="s">
         <v>202</v>
       </c>
-      <c r="D130" s="270"/>
-      <c r="E130" s="271"/>
+      <c r="D130" s="272"/>
+      <c r="E130" s="273"/>
       <c r="F130" s="167" t="s">
         <v>73</v>
       </c>
@@ -10512,13 +10512,13 @@
       <c r="O130" s="78"/>
     </row>
     <row r="131" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="264"/>
-      <c r="B131" s="298"/>
-      <c r="C131" s="269" t="s">
+      <c r="A131" s="266"/>
+      <c r="B131" s="303"/>
+      <c r="C131" s="271" t="s">
         <v>264</v>
       </c>
-      <c r="D131" s="270"/>
-      <c r="E131" s="271"/>
+      <c r="D131" s="272"/>
+      <c r="E131" s="273"/>
       <c r="F131" s="167" t="s">
         <v>73</v>
       </c>
@@ -10549,13 +10549,13 @@
       <c r="O131" s="78"/>
     </row>
     <row r="132" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="264"/>
-      <c r="B132" s="298"/>
-      <c r="C132" s="269" t="s">
+      <c r="A132" s="266"/>
+      <c r="B132" s="303"/>
+      <c r="C132" s="271" t="s">
         <v>199</v>
       </c>
-      <c r="D132" s="270"/>
-      <c r="E132" s="271"/>
+      <c r="D132" s="272"/>
+      <c r="E132" s="273"/>
       <c r="F132" s="167" t="s">
         <v>73</v>
       </c>
@@ -10586,13 +10586,13 @@
       <c r="O132" s="78"/>
     </row>
     <row r="133" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="264"/>
-      <c r="B133" s="298"/>
-      <c r="C133" s="269" t="s">
+      <c r="A133" s="266"/>
+      <c r="B133" s="303"/>
+      <c r="C133" s="271" t="s">
         <v>212</v>
       </c>
-      <c r="D133" s="270"/>
-      <c r="E133" s="271"/>
+      <c r="D133" s="272"/>
+      <c r="E133" s="273"/>
       <c r="F133" s="167" t="s">
         <v>73</v>
       </c>
@@ -10623,13 +10623,13 @@
       <c r="O133" s="78"/>
     </row>
     <row r="134" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="265"/>
-      <c r="B134" s="299"/>
-      <c r="C134" s="269" t="s">
+      <c r="A134" s="267"/>
+      <c r="B134" s="304"/>
+      <c r="C134" s="271" t="s">
         <v>213</v>
       </c>
-      <c r="D134" s="270"/>
-      <c r="E134" s="271"/>
+      <c r="D134" s="272"/>
+      <c r="E134" s="273"/>
       <c r="F134" s="167" t="s">
         <v>73</v>
       </c>
@@ -10662,9 +10662,9 @@
     <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135" s="197"/>
       <c r="B135" s="144"/>
-      <c r="C135" s="300"/>
-      <c r="D135" s="301"/>
-      <c r="E135" s="302"/>
+      <c r="C135" s="305"/>
+      <c r="D135" s="306"/>
+      <c r="E135" s="307"/>
       <c r="F135" s="118"/>
       <c r="G135" s="119"/>
       <c r="H135" s="119"/>
@@ -10681,9 +10681,9 @@
       <c r="B136" s="200"/>
       <c r="C136" s="201"/>
       <c r="D136" s="202"/>
-      <c r="E136" s="288"/>
-      <c r="F136" s="289"/>
-      <c r="G136" s="290"/>
+      <c r="E136" s="290"/>
+      <c r="F136" s="291"/>
+      <c r="G136" s="292"/>
       <c r="H136" s="165"/>
       <c r="I136" s="165"/>
       <c r="J136" s="165"/>
@@ -10698,9 +10698,9 @@
       <c r="B137" s="200"/>
       <c r="C137" s="201"/>
       <c r="D137" s="202"/>
-      <c r="E137" s="291"/>
-      <c r="F137" s="292"/>
-      <c r="G137" s="293"/>
+      <c r="E137" s="293"/>
+      <c r="F137" s="294"/>
+      <c r="G137" s="295"/>
       <c r="H137" s="165"/>
       <c r="I137" s="165"/>
       <c r="J137" s="165"/>
@@ -10714,16 +10714,16 @@
       <c r="A138" s="94" t="s">
         <v>295</v>
       </c>
-      <c r="B138" s="322">
+      <c r="B138" s="296">
         <v>42136</v>
       </c>
-      <c r="C138" s="323"/>
-      <c r="D138" s="324"/>
-      <c r="E138" s="294" t="s">
+      <c r="C138" s="297"/>
+      <c r="D138" s="298"/>
+      <c r="E138" s="299" t="s">
         <v>296</v>
       </c>
-      <c r="F138" s="295"/>
-      <c r="G138" s="296"/>
+      <c r="F138" s="300"/>
+      <c r="G138" s="301"/>
       <c r="H138" s="166"/>
       <c r="I138" s="166"/>
       <c r="J138" s="166"/>
@@ -10743,16 +10743,16 @@
       <c r="A139" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="B139" s="282" t="s">
+      <c r="B139" s="284" t="s">
         <v>33</v>
       </c>
-      <c r="C139" s="283"/>
-      <c r="D139" s="284"/>
-      <c r="E139" s="285" t="s">
+      <c r="C139" s="285"/>
+      <c r="D139" s="286"/>
+      <c r="E139" s="287" t="s">
         <v>36</v>
       </c>
-      <c r="F139" s="286"/>
-      <c r="G139" s="287"/>
+      <c r="F139" s="288"/>
+      <c r="G139" s="289"/>
       <c r="H139" s="164"/>
       <c r="I139" s="164"/>
       <c r="J139" s="164"/>
@@ -12242,7 +12242,7 @@
     <mergeCell ref="C47:E47"/>
   </mergeCells>
   <pageMargins left="1.5093749999999999" right="0.25" top="0.5" bottom="0.25" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="55" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="90" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>